<commit_message>
update for 3 paths ready for London
</commit_message>
<xml_diff>
--- a/archive-app/src/assets/data/mkGameEngine.xlsx
+++ b/archive-app/src/assets/data/mkGameEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740"/>
+    <workbookView xWindow="140" yWindow="120" windowWidth="27320" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="197">
   <si>
     <t>stage</t>
   </si>
@@ -445,6 +445,174 @@
   </si>
   <si>
     <t>5bCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>v.mc.delay</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>p3a</t>
+  </si>
+  <si>
+    <t>p3b</t>
+  </si>
+  <si>
+    <t>p3c</t>
+  </si>
+  <si>
+    <t>Path3a.mei</t>
+  </si>
+  <si>
+    <t>Path3b.mei</t>
+  </si>
+  <si>
+    <t>Path3c.mei</t>
+  </si>
+  <si>
+    <t>2a/2b</t>
+  </si>
+  <si>
+    <t>3a/3b</t>
+  </si>
+  <si>
+    <t>4b/4c/5b/5c</t>
+  </si>
+  <si>
+    <t>3b/3c/4b/4c</t>
+  </si>
+  <si>
+    <t>2a/2c/3a/3c</t>
+  </si>
+  <si>
+    <t>3cTalkativeStranger.mei</t>
+  </si>
+  <si>
+    <t>5cFallingTrees.mei</t>
+  </si>
+  <si>
+    <t>5a/5c</t>
+  </si>
+  <si>
+    <t>The performer chose the first path:5:true</t>
+  </si>
+  <si>
+    <t>The performer chose the second path:5:true</t>
+  </si>
+  <si>
+    <t>The performer chose the third path:5:true</t>
+  </si>
+  <si>
+    <t>p3aCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>1c_2</t>
+  </si>
+  <si>
+    <t>90047f</t>
+  </si>
+  <si>
+    <t>p3bCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>p3cCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>90087f</t>
+  </si>
+  <si>
+    <t>90117f</t>
+  </si>
+  <si>
+    <t>2c_1</t>
+  </si>
+  <si>
+    <t>2cCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>2c_2</t>
+  </si>
+  <si>
+    <t>BG_3c.webm</t>
+  </si>
+  <si>
+    <t>3cCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>90127f</t>
+  </si>
+  <si>
+    <t>3c_1</t>
+  </si>
+  <si>
+    <t>p1cCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>90137F</t>
+  </si>
+  <si>
+    <t>5cCustomDiskAni.webm</t>
+  </si>
+  <si>
+    <t>BG_5c.webm</t>
+  </si>
+  <si>
+    <t>BG_1c.webm</t>
+  </si>
+  <si>
+    <t>BG_2c.webm</t>
+  </si>
+  <si>
+    <t>BG_4c.webm</t>
+  </si>
+  <si>
+    <t>90147f</t>
+  </si>
+  <si>
+    <t>90157f</t>
+  </si>
+  <si>
+    <t>5c_1</t>
+  </si>
+  <si>
+    <t>BC_SP</t>
+  </si>
+  <si>
+    <t>The challenge was completed successfully:5:true</t>
+  </si>
+  <si>
+    <t>3b_1</t>
+  </si>
+  <si>
+    <t>A challenge is approaching:9:true</t>
+  </si>
+  <si>
+    <t>The performer has to choose a path:9:true</t>
+  </si>
+  <si>
+    <t>4cAnAppleTree.mei</t>
+  </si>
+  <si>
+    <t>2cHerdOfCows.mei</t>
+  </si>
+  <si>
+    <t>p3a_1</t>
+  </si>
+  <si>
+    <t>approach.png</t>
   </si>
 </sst>
 </file>
@@ -515,7 +683,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,8 +774,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -669,8 +849,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="325">
+  <cellStyleXfs count="409">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -996,8 +1185,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1053,8 +1326,29 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="325">
+  <cellStyles count="409">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1217,6 +1511,48 @@
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1379,6 +1715,48 @@
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1649,7 +2027,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1657,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB68"/>
+  <dimension ref="A1:BL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1676,47 +2054,57 @@
     <col min="9" max="9" width="9.1640625" style="11" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" style="15" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" style="15" customWidth="1"/>
-    <col min="12" max="13" width="9.83203125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" style="15" customWidth="1"/>
     <col min="14" max="14" width="5.83203125" style="15" customWidth="1"/>
     <col min="15" max="15" width="9.83203125" style="15" customWidth="1"/>
     <col min="16" max="16" width="8" style="15" customWidth="1"/>
-    <col min="17" max="17" width="17.83203125" style="15" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="15" customWidth="1"/>
     <col min="18" max="18" width="17.1640625" style="15" customWidth="1"/>
     <col min="19" max="19" width="11" style="15" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" style="7" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" style="7" customWidth="1"/>
-    <col min="23" max="23" width="7" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.33203125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="20.83203125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" style="7" customWidth="1"/>
-    <col min="27" max="27" width="9.5" style="3" customWidth="1"/>
-    <col min="28" max="28" width="11.1640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="8.33203125" style="3" customWidth="1"/>
-    <col min="30" max="30" width="6.83203125" style="3" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="3"/>
-    <col min="32" max="32" width="14.6640625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="14.83203125" style="3" customWidth="1"/>
-    <col min="34" max="34" width="9.5" style="5" customWidth="1"/>
-    <col min="35" max="35" width="11" style="5" customWidth="1"/>
-    <col min="36" max="36" width="6.83203125" style="5" customWidth="1"/>
-    <col min="37" max="37" width="6.6640625" style="5" customWidth="1"/>
-    <col min="38" max="39" width="8.83203125" style="5"/>
-    <col min="40" max="40" width="12.83203125" style="5" customWidth="1"/>
-    <col min="41" max="41" width="13" style="11" customWidth="1"/>
-    <col min="42" max="42" width="20.1640625" style="11" customWidth="1"/>
-    <col min="43" max="43" width="6.5" style="11" customWidth="1"/>
-    <col min="44" max="44" width="6.6640625" style="11" customWidth="1"/>
-    <col min="45" max="47" width="8.83203125" style="11"/>
-    <col min="48" max="48" width="20.6640625" style="11" customWidth="1"/>
-    <col min="49" max="49" width="20.1640625" style="11" customWidth="1"/>
-    <col min="50" max="50" width="6.5" style="11" customWidth="1"/>
-    <col min="51" max="51" width="6.6640625" style="11" customWidth="1"/>
-    <col min="52" max="52" width="8.83203125" style="11"/>
-    <col min="53" max="54" width="8.83203125" style="24"/>
+    <col min="20" max="20" width="10.6640625" style="15" customWidth="1"/>
+    <col min="21" max="21" width="26.6640625" style="15" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" style="7" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" style="7" customWidth="1"/>
+    <col min="25" max="26" width="7" style="7" customWidth="1"/>
+    <col min="27" max="27" width="8.33203125" style="7" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="7" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" style="7" customWidth="1"/>
+    <col min="30" max="30" width="13.1640625" style="7" customWidth="1"/>
+    <col min="31" max="31" width="38.1640625" style="7" customWidth="1"/>
+    <col min="32" max="32" width="9.5" style="3" customWidth="1"/>
+    <col min="33" max="33" width="11.1640625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="8.33203125" style="3" customWidth="1"/>
+    <col min="35" max="35" width="6.83203125" style="3" customWidth="1"/>
+    <col min="36" max="36" width="8.83203125" style="3"/>
+    <col min="37" max="37" width="14.6640625" style="3" customWidth="1"/>
+    <col min="38" max="38" width="14.83203125" style="3" customWidth="1"/>
+    <col min="39" max="39" width="11.5" style="3" customWidth="1"/>
+    <col min="40" max="40" width="38" style="3" customWidth="1"/>
+    <col min="41" max="41" width="9.5" style="5" customWidth="1"/>
+    <col min="42" max="42" width="11" style="5" customWidth="1"/>
+    <col min="43" max="43" width="6.83203125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="6.6640625" style="5" customWidth="1"/>
+    <col min="45" max="46" width="8.83203125" style="5"/>
+    <col min="47" max="47" width="12.83203125" style="5" customWidth="1"/>
+    <col min="48" max="48" width="33.5" style="5" customWidth="1"/>
+    <col min="49" max="49" width="6.83203125" style="11" customWidth="1"/>
+    <col min="50" max="50" width="20.1640625" style="11" customWidth="1"/>
+    <col min="51" max="51" width="6.5" style="11" customWidth="1"/>
+    <col min="52" max="52" width="6.6640625" style="11" customWidth="1"/>
+    <col min="53" max="55" width="8.83203125" style="11"/>
+    <col min="56" max="56" width="11.1640625" style="11" customWidth="1"/>
+    <col min="57" max="57" width="33" style="11" customWidth="1"/>
+    <col min="58" max="58" width="20.6640625" style="11" customWidth="1"/>
+    <col min="59" max="59" width="20.1640625" style="11" customWidth="1"/>
+    <col min="60" max="60" width="6.5" style="11" customWidth="1"/>
+    <col min="61" max="61" width="6.6640625" style="11" customWidth="1"/>
+    <col min="62" max="62" width="8.83203125" style="11"/>
+    <col min="63" max="64" width="8.83203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1">
+    <row r="1" spans="1:64" s="1" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1774,113 +2162,143 @@
       <c r="S1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AM1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AM1" s="18" t="s">
+      <c r="AT1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AN1" s="28" t="s">
+      <c r="AU1" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AV1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AX1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AY1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="BA1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AT1" s="26" t="s">
+      <c r="BB1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="BC1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="BD1" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="BE1" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="BA1" s="25" t="s">
+      <c r="BK1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="BB1" s="25" t="s">
+      <c r="BL1" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:64">
       <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
@@ -1924,60 +2342,86 @@
         <v>136</v>
       </c>
       <c r="S2" s="31"/>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="W2" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="36" t="s">
+      <c r="X2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
-      <c r="Z2" s="29" t="s">
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF2" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="37" t="s">
+      <c r="AG2" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="AC2" s="37" t="s">
+      <c r="AH2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="29" t="s">
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AP2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="29" t="s">
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22"/>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22"/>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-    </row>
-    <row r="3" spans="1:54">
+      <c r="AV2" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="AW2" s="11">
+        <v>6</v>
+      </c>
+      <c r="AX2" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="BD2" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="BE2" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="BF2" s="57"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+    </row>
+    <row r="3" spans="1:64">
       <c r="A3" s="32" t="s">
         <v>25</v>
       </c>
@@ -2023,54 +2467,68 @@
         <v>124</v>
       </c>
       <c r="S3" s="31"/>
-      <c r="T3" s="38" t="s">
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="W3" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="36"/>
-      <c r="W3" s="39" t="s">
+      <c r="X3" s="36"/>
+      <c r="Y3" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36" t="s">
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="Z3" s="29" t="s">
+      <c r="AC3" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="AA3" s="40" t="s">
+      <c r="AD3" s="29">
+        <v>3.1949999999999998</v>
+      </c>
+      <c r="AE3" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF3" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="AB3" s="37" t="s">
+      <c r="AG3" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AH3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="29" t="s">
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AV3" s="22"/>
-      <c r="AW3" s="22"/>
-      <c r="AX3" s="22"/>
-      <c r="AY3" s="22"/>
-      <c r="AZ3" s="22"/>
-      <c r="BA3" s="22"/>
-      <c r="BB3" s="22"/>
-    </row>
-    <row r="4" spans="1:54">
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="BF3" s="22"/>
+      <c r="BG3" s="22"/>
+      <c r="BH3" s="22"/>
+      <c r="BI3" s="22"/>
+      <c r="BJ3" s="22"/>
+      <c r="BK3" s="22"/>
+      <c r="BL3" s="22"/>
+    </row>
+    <row r="4" spans="1:64">
       <c r="A4" s="32" t="s">
         <v>4</v>
       </c>
@@ -2101,7 +2559,7 @@
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="M4" s="31" t="s">
         <v>50</v>
@@ -2119,49 +2577,67 @@
       <c r="R4" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="38" t="s">
+      <c r="S4" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T4" s="31">
+        <v>20.2</v>
+      </c>
+      <c r="U4" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V4" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="U4" s="36" t="s">
+      <c r="W4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="36" t="s">
+      <c r="X4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
       <c r="Y4" s="36"/>
-      <c r="Z4" s="29" t="s">
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29" t="s">
+        <v>189</v>
+      </c>
       <c r="AF4" s="37"/>
       <c r="AG4" s="37"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4" s="20"/>
-      <c r="AV4" s="22"/>
-      <c r="AW4" s="22"/>
-      <c r="AX4" s="22"/>
-      <c r="AY4" s="22"/>
-      <c r="AZ4" s="22"/>
-      <c r="BA4" s="22"/>
-      <c r="BB4" s="22"/>
-    </row>
-    <row r="5" spans="1:54">
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+      <c r="AN4" s="37"/>
+      <c r="AO4" s="20"/>
+      <c r="AP4" s="20"/>
+      <c r="AQ4" s="20"/>
+      <c r="AR4" s="20"/>
+      <c r="AS4" s="20"/>
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="20"/>
+      <c r="BF4" s="22"/>
+      <c r="BG4" s="22"/>
+      <c r="BH4" s="22"/>
+      <c r="BI4" s="22"/>
+      <c r="BJ4" s="22"/>
+      <c r="BK4" s="22"/>
+      <c r="BL4" s="22"/>
+    </row>
+    <row r="5" spans="1:64">
       <c r="A5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="31" t="s">
+        <v>147</v>
+      </c>
       <c r="C5" s="33" t="s">
         <v>38</v>
       </c>
@@ -2197,46 +2673,74 @@
       <c r="Q5" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="R5" s="31"/>
+      <c r="R5" s="31" t="s">
+        <v>182</v>
+      </c>
       <c r="S5" s="31"/>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="U5" s="36" t="s">
+      <c r="W5" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="36"/>
-      <c r="W5" s="39" t="s">
+      <c r="X5" s="36"/>
+      <c r="Y5" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="X5" s="36"/>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="56">
+        <v>0.5</v>
+      </c>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC5" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="37"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AV5" s="22"/>
-      <c r="AW5" s="22"/>
-      <c r="AX5" s="22"/>
-      <c r="AY5" s="22"/>
-      <c r="AZ5" s="22"/>
-      <c r="BA5" s="22"/>
-      <c r="BB5" s="22"/>
-    </row>
-    <row r="6" spans="1:54">
+      <c r="AD5" s="29">
+        <v>17</v>
+      </c>
+      <c r="AE5" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF5" s="54">
+        <v>8</v>
+      </c>
+      <c r="AG5" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH5" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI5" s="42"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="BF5" s="22"/>
+      <c r="BG5" s="22"/>
+      <c r="BH5" s="22"/>
+      <c r="BI5" s="22"/>
+      <c r="BJ5" s="22"/>
+      <c r="BK5" s="22"/>
+      <c r="BL5" s="22"/>
+    </row>
+    <row r="6" spans="1:64">
       <c r="A6" s="32" t="s">
         <v>27</v>
       </c>
@@ -2282,46 +2786,54 @@
         <v>126</v>
       </c>
       <c r="S6" s="31"/>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="U6" s="36" t="s">
+      <c r="W6" s="36" t="s">
         <v>27</v>
-      </c>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36" t="s">
-        <v>97</v>
       </c>
       <c r="X6" s="36"/>
       <c r="Y6" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="Z6" s="29" t="s">
+      <c r="AC6" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="AA6" s="37"/>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="37"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="37"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
       <c r="AF6" s="37"/>
       <c r="AG6" s="37"/>
-      <c r="AH6" s="20"/>
-      <c r="AI6" s="20"/>
-      <c r="AJ6" s="20"/>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="20"/>
-      <c r="AN6" s="20"/>
-      <c r="AV6" s="22"/>
-      <c r="AW6" s="22"/>
-      <c r="AX6" s="22"/>
-      <c r="AY6" s="22"/>
-      <c r="AZ6" s="22"/>
-      <c r="BA6" s="22"/>
-      <c r="BB6" s="22"/>
-    </row>
-    <row r="7" spans="1:54">
+      <c r="AH6" s="37"/>
+      <c r="AI6" s="37"/>
+      <c r="AJ6" s="37"/>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="37"/>
+      <c r="AN6" s="37"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="BF6" s="22"/>
+      <c r="BG6" s="22"/>
+      <c r="BH6" s="22"/>
+      <c r="BI6" s="22"/>
+      <c r="BJ6" s="22"/>
+      <c r="BK6" s="22"/>
+      <c r="BL6" s="22"/>
+    </row>
+    <row r="7" spans="1:64">
       <c r="A7" s="32" t="s">
         <v>28</v>
       </c>
@@ -2365,250 +2877,274 @@
         <v>126</v>
       </c>
       <c r="S7" s="31"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="36"/>
       <c r="W7" s="36"/>
       <c r="X7" s="36"/>
       <c r="Y7" s="36"/>
       <c r="Z7" s="36"/>
-      <c r="AA7" s="37"/>
-      <c r="AB7" s="37"/>
-      <c r="AC7" s="37"/>
-      <c r="AD7" s="37"/>
-      <c r="AE7" s="37"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="36"/>
+      <c r="AE7" s="36"/>
       <c r="AF7" s="37"/>
       <c r="AG7" s="37"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="20"/>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="20"/>
-      <c r="AN7" s="20"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="22"/>
-      <c r="AX7" s="22"/>
-      <c r="AY7" s="22"/>
-      <c r="AZ7" s="22"/>
-      <c r="BA7" s="22"/>
-      <c r="BB7" s="22"/>
-    </row>
-    <row r="8" spans="1:54">
+      <c r="AH7" s="37"/>
+      <c r="AI7" s="37"/>
+      <c r="AJ7" s="37"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="37"/>
+      <c r="AN7" s="37"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="BF7" s="22"/>
+      <c r="BG7" s="22"/>
+      <c r="BH7" s="22"/>
+      <c r="BI7" s="22"/>
+      <c r="BJ7" s="22"/>
+      <c r="BK7" s="22"/>
+      <c r="BL7" s="22"/>
+    </row>
+    <row r="8" spans="1:64">
       <c r="A8" s="32" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31" t="s">
-        <v>4</v>
+        <v>143</v>
       </c>
       <c r="M8" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="31">
-        <v>1</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>97</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
       <c r="P8" s="31"/>
       <c r="Q8" s="31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S8" s="31"/>
-      <c r="T8" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="U8" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="V8" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="W8" s="43"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="49">
+        <v>1</v>
+      </c>
+      <c r="W8" s="36" t="s">
+        <v>195</v>
+      </c>
       <c r="X8" s="36"/>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA8" s="37"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
+      <c r="Y8" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="36"/>
       <c r="AF8" s="37"/>
       <c r="AG8" s="37"/>
-      <c r="AH8" s="20"/>
-      <c r="AI8" s="20"/>
-      <c r="AJ8" s="20"/>
-      <c r="AK8" s="20"/>
-      <c r="AL8" s="20"/>
-      <c r="AM8" s="20"/>
-      <c r="AN8" s="20"/>
-      <c r="AV8" s="22"/>
-      <c r="AW8" s="22"/>
-      <c r="AX8" s="22"/>
-      <c r="AY8" s="22"/>
-      <c r="AZ8" s="22"/>
-      <c r="BA8" s="22"/>
-      <c r="BB8" s="22"/>
-    </row>
-    <row r="9" spans="1:54">
+      <c r="AH8" s="37"/>
+      <c r="AI8" s="37"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="37"/>
+      <c r="AN8" s="37"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="BF8" s="22"/>
+      <c r="BG8" s="22"/>
+      <c r="BH8" s="22"/>
+      <c r="BI8" s="22"/>
+      <c r="BJ8" s="22"/>
+      <c r="BK8" s="22"/>
+      <c r="BL8" s="22"/>
+    </row>
+    <row r="9" spans="1:64">
       <c r="A9" s="32" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
+        <v>53</v>
+      </c>
+      <c r="N9" s="31">
+        <v>1</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="S9" s="31"/>
-      <c r="T9" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="U9" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="V9" s="36"/>
+        <v>127</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T9" s="31">
+        <v>45.244999999999997</v>
+      </c>
+      <c r="U9" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V9" s="38" t="s">
+        <v>103</v>
+      </c>
       <c r="W9" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z9" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA9" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB9" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC9" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="36"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="37"/>
+      <c r="AJ9" s="37"/>
+      <c r="AK9" s="37"/>
+      <c r="AL9" s="37"/>
+      <c r="AM9" s="37"/>
+      <c r="AN9" s="37"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="20"/>
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="BF9" s="22"/>
+      <c r="BG9" s="22"/>
+      <c r="BH9" s="22"/>
+      <c r="BI9" s="22"/>
+      <c r="BJ9" s="22"/>
+      <c r="BK9" s="22"/>
+      <c r="BL9" s="22"/>
+    </row>
+    <row r="10" spans="1:64">
+      <c r="A10" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AD9" s="30"/>
-      <c r="AE9" s="37"/>
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH9" s="20"/>
-      <c r="AI9" s="20"/>
-      <c r="AJ9" s="20"/>
-      <c r="AK9" s="17"/>
-      <c r="AL9" s="20"/>
-      <c r="AM9" s="20"/>
-      <c r="AN9" s="20"/>
-      <c r="AV9" s="22"/>
-      <c r="AW9" s="22"/>
-      <c r="AX9" s="22"/>
-      <c r="AY9" s="22"/>
-      <c r="AZ9" s="22"/>
-      <c r="BA9" s="22"/>
-      <c r="BB9" s="22"/>
-    </row>
-    <row r="10" spans="1:54">
-      <c r="A10" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" s="33" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
@@ -2617,82 +3153,102 @@
         <v>115</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="S10" s="31"/>
-      <c r="T10" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="U10" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="V10" s="36"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="38" t="s">
+        <v>108</v>
+      </c>
       <c r="W10" s="36" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z10" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="36"/>
+      <c r="AB10" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC10" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="37"/>
-      <c r="AD10" s="37"/>
-      <c r="AE10" s="37"/>
-      <c r="AF10" s="37"/>
-      <c r="AG10" s="37"/>
-      <c r="AH10" s="20"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="20"/>
-      <c r="AK10" s="20"/>
-      <c r="AL10" s="20"/>
-      <c r="AM10" s="20"/>
-      <c r="AN10" s="20"/>
-      <c r="AV10" s="22"/>
-      <c r="AW10" s="22"/>
-      <c r="AX10" s="22"/>
-      <c r="AY10" s="22"/>
-      <c r="AZ10" s="22"/>
-      <c r="BA10" s="22"/>
-      <c r="BB10" s="22"/>
-    </row>
-    <row r="11" spans="1:54">
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG10" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH10" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="37"/>
+      <c r="AK10" s="37"/>
+      <c r="AL10" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="17"/>
+      <c r="AS10" s="20"/>
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="20"/>
+      <c r="BF10" s="22"/>
+      <c r="BG10" s="22"/>
+      <c r="BH10" s="22"/>
+      <c r="BI10" s="22"/>
+      <c r="BJ10" s="22"/>
+      <c r="BK10" s="22"/>
+      <c r="BL10" s="22"/>
+    </row>
+    <row r="11" spans="1:64">
       <c r="A11" s="32" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="M11" s="31"/>
+        <v>153</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>185</v>
+      </c>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
@@ -2700,126 +3256,172 @@
         <v>115</v>
       </c>
       <c r="R11" s="31" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="S11" s="31"/>
-      <c r="T11" s="36"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="53">
+        <v>2</v>
+      </c>
+      <c r="W11" s="36" t="s">
+        <v>171</v>
+      </c>
       <c r="X11" s="36"/>
-      <c r="Y11" s="36"/>
+      <c r="Y11" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="Z11" s="36"/>
-      <c r="AA11" s="37"/>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="37"/>
-      <c r="AD11" s="37"/>
-      <c r="AE11" s="37"/>
-      <c r="AF11" s="37"/>
-      <c r="AG11" s="37"/>
-      <c r="AH11" s="20"/>
-      <c r="AI11" s="20"/>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="20"/>
-      <c r="AL11" s="20"/>
-      <c r="AM11" s="20"/>
-      <c r="AN11" s="20"/>
-      <c r="AV11" s="22"/>
-      <c r="AW11" s="22"/>
-      <c r="AX11" s="22"/>
-      <c r="AY11" s="22"/>
-      <c r="AZ11" s="22"/>
-      <c r="BA11" s="22"/>
-      <c r="BB11" s="22"/>
-    </row>
-    <row r="12" spans="1:54">
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC11" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD11" s="29">
+        <v>25.536000000000001</v>
+      </c>
+      <c r="AE11" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF11" s="54">
+        <v>12</v>
+      </c>
+      <c r="AG11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH11" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="37"/>
+      <c r="AL11" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO11" s="20"/>
+      <c r="AP11" s="20"/>
+      <c r="AQ11" s="20"/>
+      <c r="AR11" s="17"/>
+      <c r="AS11" s="20"/>
+      <c r="AT11" s="20"/>
+      <c r="AU11" s="20"/>
+      <c r="AV11" s="20"/>
+      <c r="BF11" s="22"/>
+      <c r="BG11" s="22"/>
+      <c r="BH11" s="22"/>
+      <c r="BI11" s="22"/>
+      <c r="BJ11" s="22"/>
+      <c r="BK11" s="22"/>
+      <c r="BL11" s="22"/>
+    </row>
+    <row r="12" spans="1:64">
       <c r="A12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>31</v>
-      </c>
       <c r="C12" s="33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M12" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="N12" s="31">
-        <v>1</v>
-      </c>
-      <c r="O12" s="31" t="s">
-        <v>97</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R12" s="31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S12" s="31"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="W12" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
+      <c r="Y12" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="Z12" s="36"/>
-      <c r="AA12" s="40"/>
-      <c r="AB12" s="37"/>
-      <c r="AC12" s="37"/>
-      <c r="AD12" s="37"/>
-      <c r="AE12" s="37"/>
+      <c r="AA12" s="36"/>
+      <c r="AB12" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC12" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
       <c r="AF12" s="37"/>
       <c r="AG12" s="37"/>
-      <c r="AH12" s="20"/>
-      <c r="AI12" s="20"/>
-      <c r="AJ12" s="20"/>
-      <c r="AK12" s="20"/>
-      <c r="AL12" s="20"/>
-      <c r="AM12" s="20"/>
-      <c r="AN12" s="20"/>
-      <c r="AV12" s="22"/>
-      <c r="AW12" s="22"/>
-      <c r="AX12" s="22"/>
-      <c r="AY12" s="22"/>
-      <c r="AZ12" s="22"/>
-      <c r="BA12" s="22"/>
-      <c r="BB12" s="22"/>
-    </row>
-    <row r="13" spans="1:54">
+      <c r="AH12" s="37"/>
+      <c r="AI12" s="37"/>
+      <c r="AJ12" s="37"/>
+      <c r="AK12" s="37"/>
+      <c r="AL12" s="37"/>
+      <c r="AM12" s="37"/>
+      <c r="AN12" s="37"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="20"/>
+      <c r="AT12" s="20"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="20"/>
+      <c r="BF12" s="22"/>
+      <c r="BG12" s="22"/>
+      <c r="BH12" s="22"/>
+      <c r="BI12" s="22"/>
+      <c r="BJ12" s="22"/>
+      <c r="BK12" s="22"/>
+      <c r="BL12" s="22"/>
+    </row>
+    <row r="13" spans="1:64">
       <c r="A13" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>34</v>
-      </c>
       <c r="C13" s="33" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>5</v>
@@ -2842,88 +3444,92 @@
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="N13" s="31">
-        <v>1</v>
-      </c>
-      <c r="O13" s="31" t="s">
-        <v>97</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="S13" s="31"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
       <c r="V13" s="36"/>
       <c r="W13" s="36"/>
       <c r="X13" s="36"/>
       <c r="Y13" s="36"/>
       <c r="Z13" s="36"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37"/>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37"/>
-      <c r="AE13" s="37"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="36"/>
+      <c r="AD13" s="36"/>
+      <c r="AE13" s="36"/>
       <c r="AF13" s="37"/>
       <c r="AG13" s="37"/>
-      <c r="AH13" s="20"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
-      <c r="AL13" s="20"/>
-      <c r="AM13" s="20"/>
-      <c r="AN13" s="20"/>
-      <c r="AV13" s="22"/>
-      <c r="AW13" s="22"/>
-      <c r="AX13" s="22"/>
-      <c r="AY13" s="22"/>
-      <c r="AZ13" s="22"/>
-      <c r="BA13" s="22"/>
-      <c r="BB13" s="22"/>
-    </row>
-    <row r="14" spans="1:54" ht="13" customHeight="1">
+      <c r="AH13" s="37"/>
+      <c r="AI13" s="37"/>
+      <c r="AJ13" s="37"/>
+      <c r="AK13" s="37"/>
+      <c r="AL13" s="37"/>
+      <c r="AM13" s="37"/>
+      <c r="AN13" s="37"/>
+      <c r="AO13" s="20"/>
+      <c r="AP13" s="20"/>
+      <c r="AQ13" s="20"/>
+      <c r="AR13" s="20"/>
+      <c r="AS13" s="20"/>
+      <c r="AT13" s="20"/>
+      <c r="AU13" s="20"/>
+      <c r="AV13" s="20"/>
+      <c r="BF13" s="22"/>
+      <c r="BG13" s="22"/>
+      <c r="BH13" s="22"/>
+      <c r="BI13" s="22"/>
+      <c r="BJ13" s="22"/>
+      <c r="BK13" s="22"/>
+      <c r="BL13" s="22"/>
+    </row>
+    <row r="14" spans="1:64">
       <c r="A14" s="32" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="31"/>
+        <v>144</v>
+      </c>
+      <c r="M14" s="31" t="s">
+        <v>169</v>
+      </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
@@ -2934,44 +3540,62 @@
         <v>126</v>
       </c>
       <c r="S14" s="31"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="49">
+        <v>1</v>
+      </c>
+      <c r="W14" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="37"/>
-      <c r="AB14" s="37"/>
-      <c r="AC14" s="37"/>
-      <c r="AD14" s="37"/>
-      <c r="AE14" s="37"/>
+      <c r="Y14" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC14" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
       <c r="AF14" s="37"/>
       <c r="AG14" s="37"/>
-      <c r="AH14" s="20"/>
-      <c r="AI14" s="20"/>
-      <c r="AJ14" s="20"/>
-      <c r="AK14" s="20"/>
-      <c r="AL14" s="20"/>
-      <c r="AM14" s="20"/>
-      <c r="AN14" s="20"/>
-      <c r="AV14" s="22"/>
-      <c r="AW14" s="22"/>
-      <c r="AX14" s="22"/>
-      <c r="AY14" s="22"/>
-      <c r="AZ14" s="22"/>
-      <c r="BA14" s="22"/>
-      <c r="BB14" s="22"/>
-    </row>
-    <row r="15" spans="1:54">
+      <c r="AH14" s="37"/>
+      <c r="AI14" s="37"/>
+      <c r="AJ14" s="37"/>
+      <c r="AK14" s="37"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="37"/>
+      <c r="AN14" s="37"/>
+      <c r="AO14" s="20"/>
+      <c r="AP14" s="20"/>
+      <c r="AQ14" s="20"/>
+      <c r="AR14" s="20"/>
+      <c r="AS14" s="20"/>
+      <c r="AT14" s="20"/>
+      <c r="AU14" s="20"/>
+      <c r="AV14" s="20"/>
+      <c r="BF14" s="22"/>
+      <c r="BG14" s="22"/>
+      <c r="BH14" s="22"/>
+      <c r="BI14" s="22"/>
+      <c r="BJ14" s="22"/>
+      <c r="BK14" s="22"/>
+      <c r="BL14" s="22"/>
+    </row>
+    <row r="15" spans="1:64">
       <c r="A15" s="32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>5</v>
@@ -2994,57 +3618,71 @@
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
+        <v>31</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="31">
+        <v>1</v>
+      </c>
+      <c r="O15" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="P15" s="31"/>
       <c r="Q15" s="31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="S15" s="31"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
       <c r="V15" s="36"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
       <c r="Y15" s="36"/>
       <c r="Z15" s="36"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
-      <c r="AC15" s="37"/>
-      <c r="AD15" s="37"/>
-      <c r="AE15" s="37"/>
-      <c r="AF15" s="37"/>
+      <c r="AA15" s="36"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AD15" s="36"/>
+      <c r="AE15" s="36"/>
+      <c r="AF15" s="40"/>
       <c r="AG15" s="37"/>
-      <c r="AH15" s="20"/>
-      <c r="AI15" s="20"/>
-      <c r="AJ15" s="20"/>
-      <c r="AK15" s="20"/>
-      <c r="AL15" s="20"/>
-      <c r="AM15" s="20"/>
-      <c r="AN15" s="20"/>
-      <c r="AV15" s="22"/>
-      <c r="AW15" s="22"/>
-      <c r="AX15" s="22"/>
-      <c r="AY15" s="22"/>
-      <c r="AZ15" s="22"/>
-      <c r="BA15" s="22"/>
-      <c r="BB15" s="22"/>
-    </row>
-    <row r="16" spans="1:54">
+      <c r="AH15" s="37"/>
+      <c r="AI15" s="37"/>
+      <c r="AJ15" s="37"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="37"/>
+      <c r="AM15" s="37"/>
+      <c r="AN15" s="37"/>
+      <c r="AO15" s="20"/>
+      <c r="AP15" s="20"/>
+      <c r="AQ15" s="20"/>
+      <c r="AR15" s="20"/>
+      <c r="AS15" s="20"/>
+      <c r="AT15" s="20"/>
+      <c r="AU15" s="20"/>
+      <c r="AV15" s="20"/>
+      <c r="BF15" s="22"/>
+      <c r="BG15" s="22"/>
+      <c r="BH15" s="22"/>
+      <c r="BI15" s="22"/>
+      <c r="BJ15" s="22"/>
+      <c r="BK15" s="22"/>
+      <c r="BL15" s="22"/>
+    </row>
+    <row r="16" spans="1:64" ht="15" customHeight="1">
       <c r="A16" s="32" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>5</v>
@@ -3067,252 +3705,271 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
+        <v>94</v>
+      </c>
+      <c r="N16" s="31">
+        <v>1</v>
+      </c>
+      <c r="O16" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="P16" s="31"/>
       <c r="Q16" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="S16" s="31"/>
-      <c r="T16" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="U16" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="V16" s="36"/>
+        <v>130</v>
+      </c>
+      <c r="S16" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T16" s="31">
+        <v>38.331000000000003</v>
+      </c>
+      <c r="U16" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V16" s="49">
+        <v>18</v>
+      </c>
       <c r="W16" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z16" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA16" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB16" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC16" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD16" s="37"/>
-      <c r="AE16" s="37"/>
+        <v>190</v>
+      </c>
+      <c r="X16" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="36"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD16" s="36"/>
+      <c r="AE16" s="29" t="s">
+        <v>189</v>
+      </c>
       <c r="AF16" s="37"/>
-      <c r="AG16" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH16" s="44"/>
-      <c r="AI16" s="17"/>
-      <c r="AJ16" s="20"/>
-      <c r="AK16" s="20"/>
-      <c r="AL16" s="20"/>
-      <c r="AM16" s="20"/>
-      <c r="AN16" s="20"/>
-      <c r="AP16" s="16"/>
-      <c r="AR16" s="9"/>
-      <c r="AV16" s="22"/>
-      <c r="AW16" s="23"/>
-      <c r="AX16" s="22"/>
-      <c r="AY16" s="22"/>
-      <c r="AZ16" s="22"/>
-      <c r="BA16" s="22"/>
-      <c r="BB16" s="22"/>
-    </row>
-    <row r="17" spans="1:54">
+      <c r="AG16" s="37"/>
+      <c r="AH16" s="37"/>
+      <c r="AI16" s="37"/>
+      <c r="AJ16" s="37"/>
+      <c r="AK16" s="37"/>
+      <c r="AL16" s="37"/>
+      <c r="AM16" s="37"/>
+      <c r="AN16" s="37"/>
+      <c r="AO16" s="20"/>
+      <c r="AP16" s="20"/>
+      <c r="AQ16" s="20"/>
+      <c r="AR16" s="20"/>
+      <c r="AS16" s="20"/>
+      <c r="AT16" s="20"/>
+      <c r="AU16" s="20"/>
+      <c r="AV16" s="20"/>
+      <c r="BF16" s="22"/>
+      <c r="BG16" s="22"/>
+      <c r="BH16" s="22"/>
+      <c r="BI16" s="22"/>
+      <c r="BJ16" s="22"/>
+      <c r="BK16" s="22"/>
+      <c r="BL16" s="22"/>
+    </row>
+    <row r="17" spans="1:64" ht="15" customHeight="1">
       <c r="A17" s="32" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
+        <v>176</v>
+      </c>
+      <c r="N17" s="31">
+        <v>1</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="P17" s="31"/>
       <c r="Q17" s="31" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="S17" s="31"/>
-      <c r="T17" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="U17" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="V17" s="36"/>
+        <v>174</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T17" s="31">
+        <v>19.331</v>
+      </c>
+      <c r="U17" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V17" s="49">
+        <v>11</v>
+      </c>
       <c r="W17" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z17" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA17" s="37"/>
-      <c r="AB17" s="37"/>
-      <c r="AC17" s="37"/>
-      <c r="AD17" s="37"/>
-      <c r="AE17" s="37"/>
+        <v>177</v>
+      </c>
+      <c r="X17" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="36"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD17" s="36"/>
+      <c r="AE17" s="29" t="s">
+        <v>189</v>
+      </c>
       <c r="AF17" s="37"/>
       <c r="AG17" s="37"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="17"/>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
-      <c r="AL17" s="20"/>
-      <c r="AM17" s="20"/>
-      <c r="AN17" s="20"/>
-      <c r="AP17" s="16"/>
-      <c r="AV17" s="22"/>
-      <c r="AW17" s="23"/>
-      <c r="AX17" s="22"/>
-      <c r="AY17" s="22"/>
-      <c r="AZ17" s="22"/>
-      <c r="BA17" s="22"/>
-      <c r="BB17" s="22"/>
-    </row>
-    <row r="18" spans="1:54">
+      <c r="AH17" s="37"/>
+      <c r="AI17" s="37"/>
+      <c r="AJ17" s="37"/>
+      <c r="AK17" s="37"/>
+      <c r="AL17" s="37"/>
+      <c r="AM17" s="37"/>
+      <c r="AN17" s="37"/>
+      <c r="AO17" s="20"/>
+      <c r="AP17" s="20"/>
+      <c r="AQ17" s="20"/>
+      <c r="AR17" s="20"/>
+      <c r="AS17" s="20"/>
+      <c r="AT17" s="20"/>
+      <c r="AU17" s="20"/>
+      <c r="AV17" s="20"/>
+      <c r="BF17" s="22"/>
+      <c r="BG17" s="22"/>
+      <c r="BH17" s="22"/>
+      <c r="BI17" s="22"/>
+      <c r="BJ17" s="22"/>
+      <c r="BK17" s="22"/>
+      <c r="BL17" s="22"/>
+    </row>
+    <row r="18" spans="1:64" ht="13" customHeight="1">
       <c r="A18" s="32" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G18" s="34" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I18" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="N18" s="31">
-        <v>1</v>
-      </c>
-      <c r="O18" s="31" t="s">
-        <v>97</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="31" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="R18" s="31" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="S18" s="31"/>
-      <c r="T18" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="U18" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="V18" s="36" t="s">
-        <v>60</v>
-      </c>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="36"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
       <c r="Y18" s="36"/>
-      <c r="Z18" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA18" s="40"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36"/>
+      <c r="AE18" s="36"/>
       <c r="AF18" s="37"/>
       <c r="AG18" s="37"/>
-      <c r="AH18" s="20"/>
-      <c r="AI18" s="20"/>
-      <c r="AJ18" s="20"/>
-      <c r="AK18" s="20"/>
-      <c r="AL18" s="20"/>
-      <c r="AM18" s="20"/>
-      <c r="AN18" s="20"/>
-      <c r="AV18" s="22"/>
-      <c r="AW18" s="22"/>
-      <c r="AX18" s="22"/>
-      <c r="AY18" s="22"/>
-      <c r="AZ18" s="22"/>
-      <c r="BA18" s="22"/>
-      <c r="BB18" s="22"/>
-    </row>
-    <row r="19" spans="1:54">
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
+      <c r="AJ18" s="37"/>
+      <c r="AK18" s="37"/>
+      <c r="AL18" s="37"/>
+      <c r="AM18" s="37"/>
+      <c r="AN18" s="37"/>
+      <c r="AO18" s="20"/>
+      <c r="AP18" s="20"/>
+      <c r="AQ18" s="20"/>
+      <c r="AR18" s="20"/>
+      <c r="AS18" s="20"/>
+      <c r="AT18" s="20"/>
+      <c r="AU18" s="20"/>
+      <c r="AV18" s="20"/>
+      <c r="BF18" s="22"/>
+      <c r="BG18" s="22"/>
+      <c r="BH18" s="22"/>
+      <c r="BI18" s="22"/>
+      <c r="BJ18" s="22"/>
+      <c r="BK18" s="22"/>
+      <c r="BL18" s="22"/>
+    </row>
+    <row r="19" spans="1:64">
       <c r="A19" s="32" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>5</v>
@@ -3335,11 +3992,9 @@
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="31" t="s">
-        <v>49</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
@@ -3347,91 +4002,81 @@
         <v>115</v>
       </c>
       <c r="R19" s="31" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="S19" s="31"/>
-      <c r="T19" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="U19" s="36" t="s">
-        <v>87</v>
-      </c>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
       <c r="V19" s="36"/>
-      <c r="W19" s="36" t="s">
-        <v>97</v>
-      </c>
+      <c r="W19" s="36"/>
       <c r="X19" s="36"/>
-      <c r="Y19" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z19" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA19" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB19" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC19" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD19" s="30"/>
-      <c r="AE19" s="37"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
       <c r="AF19" s="37"/>
-      <c r="AG19" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH19" s="44"/>
-      <c r="AI19" s="20"/>
-      <c r="AJ19" s="20"/>
-      <c r="AK19" s="20"/>
-      <c r="AL19" s="20"/>
-      <c r="AM19" s="20"/>
-      <c r="AN19" s="20"/>
-      <c r="AV19" s="22"/>
-      <c r="AW19" s="22"/>
-      <c r="AX19" s="22"/>
-      <c r="AY19" s="22"/>
-      <c r="AZ19" s="22"/>
-      <c r="BA19" s="22"/>
-      <c r="BB19" s="22"/>
-    </row>
-    <row r="20" spans="1:54">
-      <c r="A20" s="46" t="s">
-        <v>60</v>
+      <c r="AG19" s="37"/>
+      <c r="AH19" s="37"/>
+      <c r="AI19" s="37"/>
+      <c r="AJ19" s="37"/>
+      <c r="AK19" s="37"/>
+      <c r="AL19" s="37"/>
+      <c r="AM19" s="37"/>
+      <c r="AN19" s="37"/>
+      <c r="AO19" s="20"/>
+      <c r="AP19" s="20"/>
+      <c r="AQ19" s="20"/>
+      <c r="AR19" s="20"/>
+      <c r="AS19" s="20"/>
+      <c r="AT19" s="20"/>
+      <c r="AU19" s="20"/>
+      <c r="AV19" s="20"/>
+      <c r="BF19" s="22"/>
+      <c r="BG19" s="22"/>
+      <c r="BH19" s="22"/>
+      <c r="BI19" s="22"/>
+      <c r="BJ19" s="22"/>
+      <c r="BK19" s="22"/>
+      <c r="BL19" s="22"/>
+    </row>
+    <row r="20" spans="1:64">
+      <c r="A20" s="32" t="s">
+        <v>149</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -3440,576 +4085,1307 @@
         <v>115</v>
       </c>
       <c r="R20" s="31" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="S20" s="31"/>
-      <c r="T20" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="U20" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36" t="s">
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="50">
+        <v>1</v>
+      </c>
+      <c r="W20" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z20" s="29" t="s">
+      <c r="Z20" s="52"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC20" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
+      <c r="AD20" s="36"/>
+      <c r="AE20" s="36"/>
       <c r="AF20" s="37"/>
       <c r="AG20" s="37"/>
-      <c r="AH20" s="20"/>
-      <c r="AI20" s="20"/>
-      <c r="AJ20" s="20"/>
-      <c r="AK20" s="20"/>
-      <c r="AL20" s="20"/>
-      <c r="AM20" s="20"/>
-      <c r="AN20" s="20"/>
-      <c r="AV20" s="22"/>
-      <c r="AW20" s="22"/>
-      <c r="AX20" s="22"/>
-      <c r="AY20" s="22"/>
-      <c r="AZ20" s="22"/>
-      <c r="BA20" s="22"/>
-      <c r="BB20" s="22"/>
-    </row>
-    <row r="21" spans="1:54">
+      <c r="AH20" s="37"/>
+      <c r="AI20" s="37"/>
+      <c r="AJ20" s="37"/>
+      <c r="AK20" s="37"/>
+      <c r="AL20" s="37"/>
+      <c r="AM20" s="37"/>
+      <c r="AN20" s="37"/>
+      <c r="AO20" s="20"/>
+      <c r="AP20" s="20"/>
+      <c r="AQ20" s="20"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="20"/>
+      <c r="AT20" s="20"/>
+      <c r="AU20" s="20"/>
+      <c r="AV20" s="20"/>
+      <c r="BF20" s="22"/>
+      <c r="BG20" s="22"/>
+      <c r="BH20" s="22"/>
+      <c r="BI20" s="22"/>
+      <c r="BJ20" s="22"/>
+      <c r="BK20" s="22"/>
+      <c r="BL20" s="22"/>
+    </row>
+    <row r="21" spans="1:64">
       <c r="A21" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="31"/>
+        <v>32</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>59</v>
+      </c>
       <c r="C21" s="33" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I21" s="34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+      <c r="L21" s="31" t="s">
+        <v>156</v>
+      </c>
       <c r="M21" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
+      <c r="Q21" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R21" s="31" t="s">
+        <v>131</v>
+      </c>
       <c r="S21" s="31"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="W21" s="36" t="s">
+        <v>70</v>
+      </c>
       <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
+      <c r="Y21" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="Z21" s="36"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="37"/>
-      <c r="AC21" s="37"/>
-      <c r="AD21" s="37"/>
-      <c r="AE21" s="37"/>
-      <c r="AF21" s="37"/>
-      <c r="AG21" s="37"/>
-      <c r="AH21" s="20"/>
-      <c r="AI21" s="20"/>
-      <c r="AJ21" s="20"/>
-      <c r="AK21" s="20"/>
-      <c r="AL21" s="20"/>
-      <c r="AM21" s="20"/>
-      <c r="AN21" s="20"/>
-      <c r="AV21" s="22"/>
-      <c r="AW21" s="22"/>
-      <c r="AX21" s="22"/>
-      <c r="AY21" s="22"/>
-      <c r="AZ21" s="22"/>
-      <c r="BA21" s="22"/>
-      <c r="BB21" s="22"/>
-    </row>
-    <row r="22" spans="1:54">
-      <c r="A22" s="32"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
+      <c r="AA21" s="36"/>
+      <c r="AB21" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC21" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD21" s="29">
+        <v>49.232999999999997</v>
+      </c>
+      <c r="AE21" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF21" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG21" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH21" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI21" s="37"/>
+      <c r="AJ21" s="37"/>
+      <c r="AK21" s="37"/>
+      <c r="AL21" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM21" s="30"/>
+      <c r="AN21" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO21" s="44"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="20"/>
+      <c r="AR21" s="20"/>
+      <c r="AS21" s="20"/>
+      <c r="AT21" s="20"/>
+      <c r="AU21" s="20"/>
+      <c r="AV21" s="20"/>
+      <c r="AX21" s="16"/>
+      <c r="AZ21" s="9"/>
+      <c r="BF21" s="22"/>
+      <c r="BG21" s="23"/>
+      <c r="BH21" s="22"/>
+      <c r="BI21" s="22"/>
+      <c r="BJ21" s="22"/>
+      <c r="BK21" s="22"/>
+      <c r="BL21" s="22"/>
+    </row>
+    <row r="22" spans="1:64">
+      <c r="A22" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>5</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
+      <c r="L22" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="31" t="s">
+        <v>84</v>
+      </c>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
+      <c r="Q22" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R22" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="S22" s="31"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="W22" s="36" t="s">
+        <v>109</v>
+      </c>
       <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
+      <c r="Y22" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="Z22" s="36"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="37"/>
-      <c r="AC22" s="37"/>
-      <c r="AD22" s="37"/>
-      <c r="AE22" s="37"/>
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC22" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
       <c r="AF22" s="37"/>
       <c r="AG22" s="37"/>
-      <c r="AH22" s="20"/>
-      <c r="AI22" s="20"/>
-      <c r="AJ22" s="20"/>
-      <c r="AK22" s="20"/>
-      <c r="AL22" s="20"/>
-      <c r="AM22" s="20"/>
-      <c r="AN22" s="20"/>
-      <c r="AV22" s="22"/>
-      <c r="AW22" s="22"/>
-      <c r="AX22" s="22"/>
-      <c r="AY22" s="22"/>
-      <c r="AZ22" s="22"/>
-      <c r="BA22" s="22"/>
-      <c r="BB22" s="22"/>
-    </row>
-    <row r="23" spans="1:54">
-      <c r="A23" s="32"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+      <c r="AJ22" s="37"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="37"/>
+      <c r="AM22" s="37"/>
+      <c r="AN22" s="37"/>
+      <c r="AO22" s="20"/>
+      <c r="AP22" s="17"/>
+      <c r="AQ22" s="20"/>
+      <c r="AR22" s="20"/>
+      <c r="AS22" s="20"/>
+      <c r="AT22" s="20"/>
+      <c r="AU22" s="20"/>
+      <c r="AV22" s="20"/>
+      <c r="AX22" s="16"/>
+      <c r="BF22" s="22"/>
+      <c r="BG22" s="23"/>
+      <c r="BH22" s="22"/>
+      <c r="BI22" s="22"/>
+      <c r="BJ22" s="22"/>
+      <c r="BK22" s="22"/>
+      <c r="BL22" s="22"/>
+    </row>
+    <row r="23" spans="1:64">
+      <c r="A23" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
+      <c r="L23" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="M23" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="N23" s="31">
+        <v>1</v>
+      </c>
+      <c r="O23" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
+      <c r="Q23" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R23" s="31" t="s">
+        <v>184</v>
+      </c>
       <c r="S23" s="31"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="38"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
       <c r="Y23" s="36"/>
       <c r="Z23" s="36"/>
-      <c r="AA23" s="37"/>
-      <c r="AB23" s="37"/>
-      <c r="AC23" s="37"/>
-      <c r="AD23" s="37"/>
-      <c r="AE23" s="37"/>
+      <c r="AA23" s="36"/>
+      <c r="AB23" s="36"/>
+      <c r="AC23" s="29"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="29"/>
       <c r="AF23" s="37"/>
       <c r="AG23" s="37"/>
-      <c r="AH23" s="20"/>
-      <c r="AI23" s="20"/>
-      <c r="AJ23" s="20"/>
-      <c r="AK23" s="20"/>
-      <c r="AL23" s="20"/>
-      <c r="AM23" s="20"/>
-      <c r="AN23" s="20"/>
-      <c r="AV23" s="22"/>
-      <c r="AW23" s="22"/>
-      <c r="AX23" s="22"/>
-      <c r="AY23" s="22"/>
-      <c r="AZ23" s="22"/>
-      <c r="BA23" s="22"/>
-      <c r="BB23" s="22"/>
-    </row>
-    <row r="24" spans="1:54">
-      <c r="AV24" s="22"/>
-      <c r="AW24" s="22"/>
-      <c r="AX24" s="22"/>
-      <c r="AY24" s="22"/>
-      <c r="AZ24" s="22"/>
-      <c r="BA24" s="22"/>
-      <c r="BB24" s="22"/>
-    </row>
-    <row r="25" spans="1:54">
-      <c r="AV25" s="22"/>
-      <c r="AW25" s="22"/>
-      <c r="AX25" s="22"/>
-      <c r="AY25" s="22"/>
-      <c r="AZ25" s="22"/>
-      <c r="BA25" s="22"/>
-      <c r="BB25" s="22"/>
-    </row>
-    <row r="26" spans="1:54">
-      <c r="AV26" s="22"/>
-      <c r="AW26" s="22"/>
-      <c r="AX26" s="22"/>
-      <c r="AY26" s="22"/>
-      <c r="AZ26" s="22"/>
-      <c r="BA26" s="22"/>
-      <c r="BB26" s="22"/>
-    </row>
-    <row r="27" spans="1:54">
-      <c r="AV27" s="22"/>
-      <c r="AW27" s="22"/>
-      <c r="AX27" s="22"/>
-      <c r="AY27" s="22"/>
-      <c r="AZ27" s="22"/>
-      <c r="BA27" s="22"/>
-      <c r="BB27" s="22"/>
-    </row>
-    <row r="28" spans="1:54">
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22"/>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="22"/>
-    </row>
-    <row r="29" spans="1:54">
-      <c r="AV29" s="22"/>
-      <c r="AW29" s="22"/>
-      <c r="AX29" s="22"/>
-      <c r="AY29" s="22"/>
-      <c r="AZ29" s="22"/>
-      <c r="BA29" s="22"/>
-      <c r="BB29" s="22"/>
-    </row>
-    <row r="30" spans="1:54">
-      <c r="AV30" s="22"/>
-      <c r="AW30" s="22"/>
-      <c r="AX30" s="22"/>
-      <c r="AY30" s="22"/>
-      <c r="AZ30" s="22"/>
-      <c r="BA30" s="22"/>
-      <c r="BB30" s="22"/>
-    </row>
-    <row r="31" spans="1:54">
-      <c r="AV31" s="22"/>
-      <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
-      <c r="AY31" s="22"/>
-      <c r="AZ31" s="22"/>
-      <c r="BA31" s="22"/>
-      <c r="BB31" s="22"/>
-    </row>
-    <row r="32" spans="1:54">
-      <c r="AV32" s="22"/>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="22"/>
-      <c r="AY32" s="22"/>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="22"/>
-      <c r="BB32" s="22"/>
-    </row>
-    <row r="33" spans="48:54">
-      <c r="AV33" s="19"/>
-      <c r="AW33" s="19"/>
-      <c r="AX33" s="19"/>
-      <c r="AY33" s="19"/>
-      <c r="AZ33" s="19"/>
-      <c r="BA33" s="19"/>
-      <c r="BB33" s="19"/>
-    </row>
-    <row r="34" spans="48:54">
-      <c r="AV34" s="19"/>
-      <c r="AW34" s="19"/>
-      <c r="AX34" s="19"/>
-      <c r="AY34" s="19"/>
-      <c r="AZ34" s="19"/>
-      <c r="BA34" s="19"/>
-      <c r="BB34" s="19"/>
-    </row>
-    <row r="35" spans="48:54">
-      <c r="AV35" s="19"/>
-      <c r="AW35" s="19"/>
-      <c r="AX35" s="19"/>
-      <c r="AY35" s="19"/>
-      <c r="AZ35" s="19"/>
-      <c r="BA35" s="19"/>
-      <c r="BB35" s="19"/>
-    </row>
-    <row r="36" spans="48:54">
-      <c r="AV36" s="19"/>
-      <c r="AW36" s="19"/>
-      <c r="AX36" s="19"/>
-      <c r="AY36" s="19"/>
-      <c r="AZ36" s="19"/>
-      <c r="BA36" s="19"/>
-      <c r="BB36" s="19"/>
-    </row>
-    <row r="37" spans="48:54">
-      <c r="AV37" s="19"/>
-      <c r="AW37" s="19"/>
-      <c r="AX37" s="19"/>
-      <c r="AY37" s="19"/>
-      <c r="AZ37" s="19"/>
-      <c r="BA37" s="19"/>
-      <c r="BB37" s="19"/>
-    </row>
-    <row r="38" spans="48:54">
-      <c r="AV38" s="19"/>
-      <c r="AW38" s="19"/>
-      <c r="AX38" s="19"/>
-      <c r="AY38" s="19"/>
-      <c r="AZ38" s="19"/>
-      <c r="BA38" s="19"/>
-      <c r="BB38" s="19"/>
-    </row>
-    <row r="39" spans="48:54">
-      <c r="AV39" s="19"/>
-      <c r="AW39" s="19"/>
-      <c r="AX39" s="19"/>
-      <c r="AY39" s="19"/>
-      <c r="AZ39" s="19"/>
-      <c r="BA39" s="19"/>
-      <c r="BB39" s="19"/>
-    </row>
-    <row r="40" spans="48:54">
-      <c r="AV40" s="19"/>
-      <c r="AW40" s="19"/>
-      <c r="AX40" s="19"/>
-      <c r="AY40" s="19"/>
-      <c r="AZ40" s="19"/>
-      <c r="BA40" s="19"/>
-      <c r="BB40" s="19"/>
-    </row>
-    <row r="41" spans="48:54">
-      <c r="AV41" s="19"/>
-      <c r="AW41" s="19"/>
-      <c r="AX41" s="19"/>
-      <c r="AY41" s="19"/>
-      <c r="AZ41" s="19"/>
-      <c r="BA41" s="19"/>
-      <c r="BB41" s="19"/>
-    </row>
-    <row r="42" spans="48:54">
-      <c r="AV42" s="19"/>
-      <c r="AW42" s="19"/>
-      <c r="AX42" s="19"/>
-      <c r="AY42" s="19"/>
-      <c r="AZ42" s="19"/>
-      <c r="BA42" s="19"/>
-      <c r="BB42" s="19"/>
-    </row>
-    <row r="43" spans="48:54">
-      <c r="AV43" s="19"/>
-      <c r="AW43" s="19"/>
-      <c r="AX43" s="19"/>
-      <c r="AY43" s="19"/>
-      <c r="AZ43" s="19"/>
-      <c r="BA43" s="19"/>
-      <c r="BB43" s="19"/>
-    </row>
-    <row r="44" spans="48:54">
-      <c r="AV44" s="19"/>
-      <c r="AW44" s="19"/>
-      <c r="AX44" s="19"/>
-      <c r="AY44" s="19"/>
-      <c r="AZ44" s="19"/>
-      <c r="BA44" s="19"/>
-      <c r="BB44" s="19"/>
-    </row>
-    <row r="45" spans="48:54">
-      <c r="AV45" s="19"/>
-      <c r="AW45" s="19"/>
-      <c r="AX45" s="19"/>
-      <c r="AY45" s="19"/>
-      <c r="AZ45" s="19"/>
-      <c r="BA45" s="19"/>
-      <c r="BB45" s="19"/>
-    </row>
-    <row r="46" spans="48:54">
-      <c r="AV46" s="19"/>
-      <c r="AW46" s="19"/>
-      <c r="AX46" s="19"/>
-      <c r="AY46" s="19"/>
-      <c r="AZ46" s="19"/>
-      <c r="BA46" s="19"/>
-      <c r="BB46" s="19"/>
-    </row>
-    <row r="47" spans="48:54">
-      <c r="AV47" s="19"/>
-      <c r="AW47" s="19"/>
-      <c r="AX47" s="19"/>
-      <c r="AY47" s="19"/>
-      <c r="AZ47" s="19"/>
-      <c r="BA47" s="19"/>
-      <c r="BB47" s="19"/>
-    </row>
-    <row r="48" spans="48:54">
-      <c r="AV48" s="19"/>
-      <c r="AW48" s="19"/>
-      <c r="AX48" s="19"/>
-      <c r="AY48" s="19"/>
-      <c r="AZ48" s="19"/>
-      <c r="BA48" s="19"/>
-      <c r="BB48" s="19"/>
-    </row>
-    <row r="49" spans="48:54">
-      <c r="AV49" s="19"/>
-      <c r="AW49" s="19"/>
-      <c r="AX49" s="19"/>
-      <c r="AY49" s="19"/>
-      <c r="AZ49" s="19"/>
-      <c r="BA49" s="19"/>
-      <c r="BB49" s="19"/>
-    </row>
-    <row r="50" spans="48:54">
-      <c r="AV50" s="19"/>
-      <c r="AW50" s="19"/>
-      <c r="AX50" s="19"/>
-      <c r="AY50" s="19"/>
-      <c r="AZ50" s="19"/>
-      <c r="BA50" s="19"/>
-      <c r="BB50" s="19"/>
-    </row>
-    <row r="51" spans="48:54">
-      <c r="AV51" s="19"/>
-      <c r="AW51" s="19"/>
-      <c r="AX51" s="19"/>
-      <c r="AY51" s="19"/>
-      <c r="AZ51" s="19"/>
-      <c r="BA51" s="19"/>
-      <c r="BB51" s="19"/>
-    </row>
-    <row r="52" spans="48:54">
-      <c r="AV52" s="19"/>
-      <c r="AW52" s="19"/>
-      <c r="AX52" s="19"/>
-      <c r="AY52" s="19"/>
-      <c r="AZ52" s="19"/>
-      <c r="BA52" s="19"/>
-      <c r="BB52" s="19"/>
-    </row>
-    <row r="53" spans="48:54">
-      <c r="AV53" s="19"/>
-      <c r="AW53" s="19"/>
-      <c r="AX53" s="19"/>
-      <c r="AY53" s="19"/>
-      <c r="AZ53" s="19"/>
-      <c r="BA53" s="19"/>
-      <c r="BB53" s="19"/>
-    </row>
-    <row r="54" spans="48:54">
-      <c r="AV54" s="19"/>
-      <c r="AW54" s="19"/>
-      <c r="AX54" s="19"/>
-      <c r="AY54" s="19"/>
-      <c r="AZ54" s="19"/>
-      <c r="BA54" s="19"/>
-      <c r="BB54" s="19"/>
-    </row>
-    <row r="55" spans="48:54">
-      <c r="AV55" s="19"/>
-      <c r="AW55" s="19"/>
-      <c r="AX55" s="19"/>
-      <c r="AY55" s="19"/>
-      <c r="AZ55" s="19"/>
-      <c r="BA55" s="19"/>
-      <c r="BB55" s="19"/>
-    </row>
-    <row r="56" spans="48:54">
-      <c r="AV56" s="19"/>
-      <c r="AW56" s="19"/>
-      <c r="AX56" s="19"/>
-      <c r="AY56" s="19"/>
-      <c r="AZ56" s="19"/>
-      <c r="BA56" s="19"/>
-      <c r="BB56" s="19"/>
-    </row>
-    <row r="57" spans="48:54">
-      <c r="AV57" s="19"/>
-      <c r="AW57" s="19"/>
-      <c r="AX57" s="19"/>
-      <c r="AY57" s="19"/>
-      <c r="AZ57" s="19"/>
-      <c r="BA57" s="19"/>
-      <c r="BB57" s="19"/>
-    </row>
-    <row r="58" spans="48:54">
-      <c r="AV58" s="19"/>
-      <c r="AW58" s="19"/>
-      <c r="AX58" s="19"/>
-      <c r="AY58" s="19"/>
-      <c r="AZ58" s="19"/>
-      <c r="BA58" s="19"/>
-      <c r="BB58" s="19"/>
-    </row>
-    <row r="59" spans="48:54">
-      <c r="AV59" s="19"/>
-      <c r="AW59" s="19"/>
-      <c r="AX59" s="19"/>
-      <c r="AY59" s="19"/>
-      <c r="AZ59" s="19"/>
-      <c r="BA59" s="19"/>
-      <c r="BB59" s="19"/>
-    </row>
-    <row r="60" spans="48:54">
-      <c r="BA60" s="11"/>
-      <c r="BB60" s="11"/>
-    </row>
-    <row r="61" spans="48:54">
-      <c r="BA61" s="11"/>
-      <c r="BB61" s="11"/>
-    </row>
-    <row r="62" spans="48:54">
-      <c r="BA62" s="11"/>
-      <c r="BB62" s="11"/>
-    </row>
-    <row r="63" spans="48:54">
-      <c r="BA63" s="11"/>
-      <c r="BB63" s="11"/>
-    </row>
-    <row r="64" spans="48:54">
-      <c r="BA64" s="11"/>
-      <c r="BB64" s="11"/>
-    </row>
-    <row r="65" spans="53:54">
-      <c r="BA65" s="11"/>
-      <c r="BB65" s="11"/>
-    </row>
-    <row r="66" spans="53:54">
-      <c r="BA66" s="11"/>
-      <c r="BB66" s="11"/>
-    </row>
-    <row r="67" spans="53:54">
-      <c r="BA67" s="11"/>
-      <c r="BB67" s="11"/>
-    </row>
-    <row r="68" spans="53:54">
-      <c r="BA68" s="11"/>
-      <c r="BB68" s="11"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
+      <c r="AJ23" s="37"/>
+      <c r="AK23" s="37"/>
+      <c r="AL23" s="37"/>
+      <c r="AM23" s="37"/>
+      <c r="AN23" s="37"/>
+      <c r="AO23" s="20"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="20"/>
+      <c r="AR23" s="20"/>
+      <c r="AS23" s="20"/>
+      <c r="AT23" s="20"/>
+      <c r="AU23" s="20"/>
+      <c r="AV23" s="20"/>
+      <c r="AX23" s="16"/>
+      <c r="BF23" s="22"/>
+      <c r="BG23" s="23"/>
+      <c r="BH23" s="22"/>
+      <c r="BI23" s="22"/>
+      <c r="BJ23" s="22"/>
+      <c r="BK23" s="22"/>
+      <c r="BL23" s="22"/>
+    </row>
+    <row r="24" spans="1:64">
+      <c r="A24" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="M24" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" s="31">
+        <v>1</v>
+      </c>
+      <c r="O24" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="R24" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="S24" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T24" s="31">
+        <v>33.22</v>
+      </c>
+      <c r="U24" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V24" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="W24" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="X24" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="36"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF24" s="40"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="37"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="20"/>
+      <c r="AP24" s="20"/>
+      <c r="AQ24" s="20"/>
+      <c r="AR24" s="20"/>
+      <c r="AS24" s="20"/>
+      <c r="AT24" s="20"/>
+      <c r="AU24" s="20"/>
+      <c r="AV24" s="20"/>
+      <c r="BF24" s="22"/>
+      <c r="BG24" s="22"/>
+      <c r="BH24" s="22"/>
+      <c r="BI24" s="22"/>
+      <c r="BJ24" s="22"/>
+      <c r="BK24" s="22"/>
+      <c r="BL24" s="22"/>
+    </row>
+    <row r="25" spans="1:64">
+      <c r="A25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="M25" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R25" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="W25" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z25" s="36"/>
+      <c r="AA25" s="36"/>
+      <c r="AB25" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC25" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD25" s="29">
+        <v>1.298</v>
+      </c>
+      <c r="AE25" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF25" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG25" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH25" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI25" s="30"/>
+      <c r="AJ25" s="37"/>
+      <c r="AK25" s="37"/>
+      <c r="AL25" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM25" s="30"/>
+      <c r="AN25" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO25" s="44"/>
+      <c r="AP25" s="20"/>
+      <c r="AQ25" s="20"/>
+      <c r="AR25" s="20"/>
+      <c r="AS25" s="20"/>
+      <c r="AT25" s="20"/>
+      <c r="AU25" s="20"/>
+      <c r="AV25" s="20"/>
+      <c r="BF25" s="22"/>
+      <c r="BG25" s="22"/>
+      <c r="BH25" s="22"/>
+      <c r="BI25" s="22"/>
+      <c r="BJ25" s="22"/>
+      <c r="BK25" s="22"/>
+      <c r="BL25" s="22"/>
+    </row>
+    <row r="26" spans="1:64">
+      <c r="A26" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M26" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="N26" s="31">
+        <v>1</v>
+      </c>
+      <c r="O26" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="R26" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S26" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="T26" s="31">
+        <v>55.5</v>
+      </c>
+      <c r="U26" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="V26" s="53">
+        <v>25</v>
+      </c>
+      <c r="W26" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="X26" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
+      <c r="AA26" s="36"/>
+      <c r="AB26" s="36"/>
+      <c r="AC26" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF26" s="40"/>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="37"/>
+      <c r="AI26" s="30"/>
+      <c r="AJ26" s="37"/>
+      <c r="AK26" s="37"/>
+      <c r="AL26" s="30"/>
+      <c r="AM26" s="30"/>
+      <c r="AN26" s="30"/>
+      <c r="AO26" s="44"/>
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="20"/>
+      <c r="AR26" s="20"/>
+      <c r="AS26" s="20"/>
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="BF26" s="22"/>
+      <c r="BG26" s="22"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="22"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="22"/>
+      <c r="BL26" s="22"/>
+    </row>
+    <row r="27" spans="1:64">
+      <c r="A27" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R27" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="W27" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z27" s="36"/>
+      <c r="AA27" s="36"/>
+      <c r="AB27" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC27" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="37"/>
+      <c r="AG27" s="37"/>
+      <c r="AH27" s="37"/>
+      <c r="AI27" s="37"/>
+      <c r="AJ27" s="37"/>
+      <c r="AK27" s="37"/>
+      <c r="AL27" s="37"/>
+      <c r="AM27" s="37"/>
+      <c r="AN27" s="37"/>
+      <c r="AO27" s="20"/>
+      <c r="AP27" s="20"/>
+      <c r="AQ27" s="20"/>
+      <c r="AR27" s="20"/>
+      <c r="AS27" s="20"/>
+      <c r="AT27" s="20"/>
+      <c r="AU27" s="20"/>
+      <c r="AV27" s="20"/>
+      <c r="BF27" s="22"/>
+      <c r="BG27" s="22"/>
+      <c r="BH27" s="22"/>
+      <c r="BI27" s="22"/>
+      <c r="BJ27" s="22"/>
+      <c r="BK27" s="22"/>
+      <c r="BL27" s="22"/>
+    </row>
+    <row r="28" spans="1:64">
+      <c r="A28" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="31"/>
+      <c r="C28" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
+      <c r="X28" s="36"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="36"/>
+      <c r="AA28" s="36"/>
+      <c r="AB28" s="36"/>
+      <c r="AC28" s="36"/>
+      <c r="AD28" s="36"/>
+      <c r="AE28" s="36"/>
+      <c r="AF28" s="37"/>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
+      <c r="AM28" s="37"/>
+      <c r="AN28" s="37"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20"/>
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22"/>
+      <c r="BL28" s="22"/>
+    </row>
+    <row r="29" spans="1:64">
+      <c r="A29" s="32"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AA29" s="36"/>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="37"/>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="37"/>
+      <c r="AI29" s="37"/>
+      <c r="AJ29" s="37"/>
+      <c r="AK29" s="37"/>
+      <c r="AL29" s="37"/>
+      <c r="AM29" s="37"/>
+      <c r="AN29" s="37"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20"/>
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="BF29" s="22"/>
+      <c r="BG29" s="22"/>
+      <c r="BH29" s="22"/>
+      <c r="BI29" s="22"/>
+      <c r="BJ29" s="22"/>
+      <c r="BK29" s="22"/>
+      <c r="BL29" s="22"/>
+    </row>
+    <row r="30" spans="1:64">
+      <c r="A30" s="32"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="37"/>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="37"/>
+      <c r="AJ30" s="37"/>
+      <c r="AK30" s="37"/>
+      <c r="AL30" s="37"/>
+      <c r="AM30" s="37"/>
+      <c r="AN30" s="37"/>
+      <c r="AO30" s="20"/>
+      <c r="AP30" s="20"/>
+      <c r="AQ30" s="20"/>
+      <c r="AR30" s="20"/>
+      <c r="AS30" s="20"/>
+      <c r="AT30" s="20"/>
+      <c r="AU30" s="20"/>
+      <c r="AV30" s="20"/>
+      <c r="BF30" s="22"/>
+      <c r="BG30" s="22"/>
+      <c r="BH30" s="22"/>
+      <c r="BI30" s="22"/>
+      <c r="BJ30" s="22"/>
+      <c r="BK30" s="22"/>
+      <c r="BL30" s="22"/>
+    </row>
+    <row r="31" spans="1:64">
+      <c r="BF31" s="22"/>
+      <c r="BG31" s="22"/>
+      <c r="BH31" s="22"/>
+      <c r="BI31" s="22"/>
+      <c r="BJ31" s="22"/>
+      <c r="BK31" s="22"/>
+      <c r="BL31" s="22"/>
+    </row>
+    <row r="32" spans="1:64">
+      <c r="BF32" s="22"/>
+      <c r="BG32" s="22"/>
+      <c r="BH32" s="22"/>
+      <c r="BI32" s="22"/>
+      <c r="BJ32" s="22"/>
+      <c r="BK32" s="22"/>
+      <c r="BL32" s="22"/>
+    </row>
+    <row r="33" spans="58:64">
+      <c r="BF33" s="22"/>
+      <c r="BG33" s="22"/>
+      <c r="BH33" s="22"/>
+      <c r="BI33" s="22"/>
+      <c r="BJ33" s="22"/>
+      <c r="BK33" s="22"/>
+      <c r="BL33" s="22"/>
+    </row>
+    <row r="34" spans="58:64">
+      <c r="BF34" s="22"/>
+      <c r="BG34" s="22"/>
+      <c r="BH34" s="22"/>
+      <c r="BI34" s="22"/>
+      <c r="BJ34" s="22"/>
+      <c r="BK34" s="22"/>
+      <c r="BL34" s="22"/>
+    </row>
+    <row r="35" spans="58:64">
+      <c r="BF35" s="22"/>
+      <c r="BG35" s="22"/>
+      <c r="BH35" s="22"/>
+      <c r="BI35" s="22"/>
+      <c r="BJ35" s="22"/>
+      <c r="BK35" s="22"/>
+      <c r="BL35" s="22"/>
+    </row>
+    <row r="36" spans="58:64">
+      <c r="BF36" s="22"/>
+      <c r="BG36" s="22"/>
+      <c r="BH36" s="22"/>
+      <c r="BI36" s="22"/>
+      <c r="BJ36" s="22"/>
+      <c r="BK36" s="22"/>
+      <c r="BL36" s="22"/>
+    </row>
+    <row r="37" spans="58:64">
+      <c r="BF37" s="22"/>
+      <c r="BG37" s="22"/>
+      <c r="BH37" s="22"/>
+      <c r="BI37" s="22"/>
+      <c r="BJ37" s="22"/>
+      <c r="BK37" s="22"/>
+      <c r="BL37" s="22"/>
+    </row>
+    <row r="38" spans="58:64">
+      <c r="BF38" s="22"/>
+      <c r="BG38" s="22"/>
+      <c r="BH38" s="22"/>
+      <c r="BI38" s="22"/>
+      <c r="BJ38" s="22"/>
+      <c r="BK38" s="22"/>
+      <c r="BL38" s="22"/>
+    </row>
+    <row r="39" spans="58:64">
+      <c r="BF39" s="22"/>
+      <c r="BG39" s="22"/>
+      <c r="BH39" s="22"/>
+      <c r="BI39" s="22"/>
+      <c r="BJ39" s="22"/>
+      <c r="BK39" s="22"/>
+      <c r="BL39" s="22"/>
+    </row>
+    <row r="40" spans="58:64">
+      <c r="BF40" s="19"/>
+      <c r="BG40" s="19"/>
+      <c r="BH40" s="19"/>
+      <c r="BI40" s="19"/>
+      <c r="BJ40" s="19"/>
+      <c r="BK40" s="19"/>
+      <c r="BL40" s="19"/>
+    </row>
+    <row r="41" spans="58:64">
+      <c r="BF41" s="19"/>
+      <c r="BG41" s="19"/>
+      <c r="BH41" s="19"/>
+      <c r="BI41" s="19"/>
+      <c r="BJ41" s="19"/>
+      <c r="BK41" s="19"/>
+      <c r="BL41" s="19"/>
+    </row>
+    <row r="42" spans="58:64">
+      <c r="BF42" s="19"/>
+      <c r="BG42" s="19"/>
+      <c r="BH42" s="19"/>
+      <c r="BI42" s="19"/>
+      <c r="BJ42" s="19"/>
+      <c r="BK42" s="19"/>
+      <c r="BL42" s="19"/>
+    </row>
+    <row r="43" spans="58:64">
+      <c r="BF43" s="19"/>
+      <c r="BG43" s="19"/>
+      <c r="BH43" s="19"/>
+      <c r="BI43" s="19"/>
+      <c r="BJ43" s="19"/>
+      <c r="BK43" s="19"/>
+      <c r="BL43" s="19"/>
+    </row>
+    <row r="44" spans="58:64">
+      <c r="BF44" s="19"/>
+      <c r="BG44" s="19"/>
+      <c r="BH44" s="19"/>
+      <c r="BI44" s="19"/>
+      <c r="BJ44" s="19"/>
+      <c r="BK44" s="19"/>
+      <c r="BL44" s="19"/>
+    </row>
+    <row r="45" spans="58:64">
+      <c r="BF45" s="19"/>
+      <c r="BG45" s="19"/>
+      <c r="BH45" s="19"/>
+      <c r="BI45" s="19"/>
+      <c r="BJ45" s="19"/>
+      <c r="BK45" s="19"/>
+      <c r="BL45" s="19"/>
+    </row>
+    <row r="46" spans="58:64">
+      <c r="BF46" s="19"/>
+      <c r="BG46" s="19"/>
+      <c r="BH46" s="19"/>
+      <c r="BI46" s="19"/>
+      <c r="BJ46" s="19"/>
+      <c r="BK46" s="19"/>
+      <c r="BL46" s="19"/>
+    </row>
+    <row r="47" spans="58:64">
+      <c r="BF47" s="19"/>
+      <c r="BG47" s="19"/>
+      <c r="BH47" s="19"/>
+      <c r="BI47" s="19"/>
+      <c r="BJ47" s="19"/>
+      <c r="BK47" s="19"/>
+      <c r="BL47" s="19"/>
+    </row>
+    <row r="48" spans="58:64">
+      <c r="BF48" s="19"/>
+      <c r="BG48" s="19"/>
+      <c r="BH48" s="19"/>
+      <c r="BI48" s="19"/>
+      <c r="BJ48" s="19"/>
+      <c r="BK48" s="19"/>
+      <c r="BL48" s="19"/>
+    </row>
+    <row r="49" spans="58:64">
+      <c r="BF49" s="19"/>
+      <c r="BG49" s="19"/>
+      <c r="BH49" s="19"/>
+      <c r="BI49" s="19"/>
+      <c r="BJ49" s="19"/>
+      <c r="BK49" s="19"/>
+      <c r="BL49" s="19"/>
+    </row>
+    <row r="50" spans="58:64">
+      <c r="BF50" s="19"/>
+      <c r="BG50" s="19"/>
+      <c r="BH50" s="19"/>
+      <c r="BI50" s="19"/>
+      <c r="BJ50" s="19"/>
+      <c r="BK50" s="19"/>
+      <c r="BL50" s="19"/>
+    </row>
+    <row r="51" spans="58:64">
+      <c r="BF51" s="19"/>
+      <c r="BG51" s="19"/>
+      <c r="BH51" s="19"/>
+      <c r="BI51" s="19"/>
+      <c r="BJ51" s="19"/>
+      <c r="BK51" s="19"/>
+      <c r="BL51" s="19"/>
+    </row>
+    <row r="52" spans="58:64">
+      <c r="BF52" s="19"/>
+      <c r="BG52" s="19"/>
+      <c r="BH52" s="19"/>
+      <c r="BI52" s="19"/>
+      <c r="BJ52" s="19"/>
+      <c r="BK52" s="19"/>
+      <c r="BL52" s="19"/>
+    </row>
+    <row r="53" spans="58:64">
+      <c r="BF53" s="19"/>
+      <c r="BG53" s="19"/>
+      <c r="BH53" s="19"/>
+      <c r="BI53" s="19"/>
+      <c r="BJ53" s="19"/>
+      <c r="BK53" s="19"/>
+      <c r="BL53" s="19"/>
+    </row>
+    <row r="54" spans="58:64">
+      <c r="BF54" s="19"/>
+      <c r="BG54" s="19"/>
+      <c r="BH54" s="19"/>
+      <c r="BI54" s="19"/>
+      <c r="BJ54" s="19"/>
+      <c r="BK54" s="19"/>
+      <c r="BL54" s="19"/>
+    </row>
+    <row r="55" spans="58:64">
+      <c r="BF55" s="19"/>
+      <c r="BG55" s="19"/>
+      <c r="BH55" s="19"/>
+      <c r="BI55" s="19"/>
+      <c r="BJ55" s="19"/>
+      <c r="BK55" s="19"/>
+      <c r="BL55" s="19"/>
+    </row>
+    <row r="56" spans="58:64">
+      <c r="BF56" s="19"/>
+      <c r="BG56" s="19"/>
+      <c r="BH56" s="19"/>
+      <c r="BI56" s="19"/>
+      <c r="BJ56" s="19"/>
+      <c r="BK56" s="19"/>
+      <c r="BL56" s="19"/>
+    </row>
+    <row r="57" spans="58:64">
+      <c r="BF57" s="19"/>
+      <c r="BG57" s="19"/>
+      <c r="BH57" s="19"/>
+      <c r="BI57" s="19"/>
+      <c r="BJ57" s="19"/>
+      <c r="BK57" s="19"/>
+      <c r="BL57" s="19"/>
+    </row>
+    <row r="58" spans="58:64">
+      <c r="BF58" s="19"/>
+      <c r="BG58" s="19"/>
+      <c r="BH58" s="19"/>
+      <c r="BI58" s="19"/>
+      <c r="BJ58" s="19"/>
+      <c r="BK58" s="19"/>
+      <c r="BL58" s="19"/>
+    </row>
+    <row r="59" spans="58:64">
+      <c r="BF59" s="19"/>
+      <c r="BG59" s="19"/>
+      <c r="BH59" s="19"/>
+      <c r="BI59" s="19"/>
+      <c r="BJ59" s="19"/>
+      <c r="BK59" s="19"/>
+      <c r="BL59" s="19"/>
+    </row>
+    <row r="60" spans="58:64">
+      <c r="BF60" s="19"/>
+      <c r="BG60" s="19"/>
+      <c r="BH60" s="19"/>
+      <c r="BI60" s="19"/>
+      <c r="BJ60" s="19"/>
+      <c r="BK60" s="19"/>
+      <c r="BL60" s="19"/>
+    </row>
+    <row r="61" spans="58:64">
+      <c r="BF61" s="19"/>
+      <c r="BG61" s="19"/>
+      <c r="BH61" s="19"/>
+      <c r="BI61" s="19"/>
+      <c r="BJ61" s="19"/>
+      <c r="BK61" s="19"/>
+      <c r="BL61" s="19"/>
+    </row>
+    <row r="62" spans="58:64">
+      <c r="BF62" s="19"/>
+      <c r="BG62" s="19"/>
+      <c r="BH62" s="19"/>
+      <c r="BI62" s="19"/>
+      <c r="BJ62" s="19"/>
+      <c r="BK62" s="19"/>
+      <c r="BL62" s="19"/>
+    </row>
+    <row r="63" spans="58:64">
+      <c r="BF63" s="19"/>
+      <c r="BG63" s="19"/>
+      <c r="BH63" s="19"/>
+      <c r="BI63" s="19"/>
+      <c r="BJ63" s="19"/>
+      <c r="BK63" s="19"/>
+      <c r="BL63" s="19"/>
+    </row>
+    <row r="64" spans="58:64">
+      <c r="BF64" s="19"/>
+      <c r="BG64" s="19"/>
+      <c r="BH64" s="19"/>
+      <c r="BI64" s="19"/>
+      <c r="BJ64" s="19"/>
+      <c r="BK64" s="19"/>
+      <c r="BL64" s="19"/>
+    </row>
+    <row r="65" spans="58:64">
+      <c r="BF65" s="19"/>
+      <c r="BG65" s="19"/>
+      <c r="BH65" s="19"/>
+      <c r="BI65" s="19"/>
+      <c r="BJ65" s="19"/>
+      <c r="BK65" s="19"/>
+      <c r="BL65" s="19"/>
+    </row>
+    <row r="66" spans="58:64">
+      <c r="BF66" s="19"/>
+      <c r="BG66" s="19"/>
+      <c r="BH66" s="19"/>
+      <c r="BI66" s="19"/>
+      <c r="BJ66" s="19"/>
+      <c r="BK66" s="19"/>
+      <c r="BL66" s="19"/>
+    </row>
+    <row r="67" spans="58:64">
+      <c r="BK67" s="11"/>
+      <c r="BL67" s="11"/>
+    </row>
+    <row r="68" spans="58:64">
+      <c r="BK68" s="11"/>
+      <c r="BL68" s="11"/>
+    </row>
+    <row r="69" spans="58:64">
+      <c r="BK69" s="11"/>
+      <c r="BL69" s="11"/>
+    </row>
+    <row r="70" spans="58:64">
+      <c r="BK70" s="11"/>
+      <c r="BL70" s="11"/>
+    </row>
+    <row r="71" spans="58:64">
+      <c r="BK71" s="11"/>
+      <c r="BL71" s="11"/>
+    </row>
+    <row r="72" spans="58:64">
+      <c r="BK72" s="11"/>
+      <c r="BL72" s="11"/>
+    </row>
+    <row r="73" spans="58:64">
+      <c r="BK73" s="11"/>
+      <c r="BL73" s="11"/>
+    </row>
+    <row r="74" spans="58:64">
+      <c r="BK74" s="11"/>
+      <c r="BL74" s="11"/>
+    </row>
+    <row r="75" spans="58:64">
+      <c r="BK75" s="11"/>
+      <c r="BL75" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="AC5:AE6">
-    <sortCondition descending="1" ref="AE5"/>
+  <sortState ref="AH5:AJ6">
+    <sortCondition descending="1" ref="AJ5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update config files; fix narrative text extraction defaults
</commit_message>
<xml_diff>
--- a/archive-app/src/assets/data/mkGameEngine.xlsx
+++ b/archive-app/src/assets/data/mkGameEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="120" windowWidth="27320" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="193">
   <si>
     <t>stage</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Ending 1</t>
   </si>
   <si>
-    <t>Ending 2</t>
-  </si>
-  <si>
     <t>Ending 3</t>
   </si>
   <si>
@@ -489,15 +486,6 @@
     <t>3a/3b</t>
   </si>
   <si>
-    <t>4b/4c/5b/5c</t>
-  </si>
-  <si>
-    <t>3b/3c/4b/4c</t>
-  </si>
-  <si>
-    <t>2a/2c/3a/3c</t>
-  </si>
-  <si>
     <t>3cTalkativeStranger.mei</t>
   </si>
   <si>
@@ -528,9 +516,6 @@
     <t>p3bCustomDiskAni.webm</t>
   </si>
   <si>
-    <t>p3cCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>90087f</t>
   </si>
   <si>
@@ -540,33 +525,21 @@
     <t>2c_1</t>
   </si>
   <si>
-    <t>2cCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>2c_2</t>
   </si>
   <si>
     <t>BG_3c.webm</t>
   </si>
   <si>
-    <t>3cCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>90127f</t>
   </si>
   <si>
     <t>3c_1</t>
   </si>
   <si>
-    <t>p1cCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>90137F</t>
   </si>
   <si>
-    <t>5cCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>BG_5c.webm</t>
   </si>
   <si>
@@ -612,7 +585,22 @@
     <t>p3a_1</t>
   </si>
   <si>
-    <t>approach.png</t>
+    <t>3a/3c</t>
+  </si>
+  <si>
+    <t>4b/4c</t>
+  </si>
+  <si>
+    <t>5b/5c</t>
+  </si>
+  <si>
+    <t>approach.webm</t>
+  </si>
+  <si>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>Ending 2,12</t>
   </si>
 </sst>
 </file>
@@ -859,8 +847,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="409">
+  <cellStyleXfs count="411">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1348,7 +1338,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="409">
+  <cellStyles count="411">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1553,6 +1543,7 @@
     <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1757,6 +1748,7 @@
     <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2027,7 +2019,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2037,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2109,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -2145,28 +2137,28 @@
         <v>20</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P1" s="14" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>63</v>
-      </c>
       <c r="T1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>18</v>
@@ -2181,22 +2173,22 @@
         <v>20</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AB1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="AD1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>16</v>
@@ -2214,16 +2206,16 @@
         <v>15</v>
       </c>
       <c r="AK1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="AM1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="AO1" s="4" t="s">
         <v>19</v>
@@ -2241,16 +2233,16 @@
         <v>15</v>
       </c>
       <c r="AT1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" s="28" t="s">
-        <v>63</v>
-      </c>
       <c r="AV1" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AW1" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AX1" s="9" t="s">
         <v>17</v>
@@ -2265,19 +2257,19 @@
         <v>15</v>
       </c>
       <c r="BB1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="BC1" s="27" t="s">
-        <v>63</v>
-      </c>
       <c r="BD1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="BE1" s="27" t="s">
-        <v>142</v>
-      </c>
       <c r="BF1" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BG1" s="21" t="s">
         <v>17</v>
@@ -2292,10 +2284,10 @@
         <v>15</v>
       </c>
       <c r="BK1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="BL1" s="25" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:64">
@@ -2303,10 +2295,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>5</v>
@@ -2329,17 +2321,17 @@
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="35"/>
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
       <c r="P2" s="31"/>
       <c r="Q2" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
@@ -2348,27 +2340,27 @@
         <v>22</v>
       </c>
       <c r="W2" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X2" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="36"/>
       <c r="Z2" s="36"/>
       <c r="AA2" s="36"/>
       <c r="AB2" s="36"/>
       <c r="AC2" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD2" s="29"/>
       <c r="AE2" s="29" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AF2" s="37" t="s">
-        <v>23</v>
+        <v>192</v>
       </c>
       <c r="AG2" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AH2" s="37" t="s">
         <v>4</v>
@@ -2377,17 +2369,17 @@
       <c r="AJ2" s="37"/>
       <c r="AK2" s="37"/>
       <c r="AL2" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM2" s="30"/>
       <c r="AN2" s="30" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="AO2" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AP2" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AQ2" s="20" t="s">
         <v>6</v>
@@ -2396,22 +2388,22 @@
       <c r="AS2" s="20"/>
       <c r="AT2" s="20"/>
       <c r="AU2" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AV2" s="48" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AW2" s="11">
         <v>6</v>
       </c>
       <c r="AX2" s="11" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="BD2" s="11">
         <v>3.6</v>
       </c>
       <c r="BE2" s="16" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="BF2" s="57"/>
       <c r="BG2" s="22"/>
@@ -2423,13 +2415,13 @@
     </row>
     <row r="3" spans="1:64">
       <c r="A3" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>5</v>
@@ -2452,65 +2444,65 @@
       <c r="J3" s="31"/>
       <c r="K3" s="31"/>
       <c r="L3" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
       <c r="P3" s="31"/>
       <c r="Q3" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R3" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S3" s="31"/>
       <c r="T3" s="31"/>
       <c r="U3" s="31"/>
       <c r="V3" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W3" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X3" s="36"/>
       <c r="Y3" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="56"/>
       <c r="AA3" s="36"/>
       <c r="AB3" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC3" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD3" s="29">
         <v>3.1949999999999998</v>
       </c>
       <c r="AE3" s="48" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AF3" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG3" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH3" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI3" s="37"/>
       <c r="AJ3" s="37"/>
       <c r="AK3" s="37"/>
       <c r="AL3" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM3" s="30"/>
       <c r="AN3" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO3" s="20"/>
       <c r="AP3" s="20"/>
@@ -2533,10 +2525,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>3</v>
@@ -2562,49 +2554,49 @@
         <v>6</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N4" s="31">
         <v>1</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T4" s="31">
         <v>20.2</v>
       </c>
       <c r="U4" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V4" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W4" s="36" t="s">
         <v>4</v>
       </c>
       <c r="X4" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y4" s="36"/>
       <c r="Z4" s="36"/>
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD4" s="29"/>
       <c r="AE4" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF4" s="37"/>
       <c r="AG4" s="37"/>
@@ -2636,10 +2628,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>3</v>
@@ -2662,67 +2654,65 @@
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
       <c r="Q5" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="S5" s="31"/>
       <c r="T5" s="31"/>
       <c r="U5" s="31"/>
       <c r="V5" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W5" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X5" s="36"/>
       <c r="Y5" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z5" s="56">
         <v>0.5</v>
       </c>
       <c r="AA5" s="36"/>
-      <c r="AB5" s="36" t="s">
-        <v>178</v>
-      </c>
+      <c r="AB5" s="36"/>
       <c r="AC5" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD5" s="29">
         <v>17</v>
       </c>
       <c r="AE5" s="48" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AF5" s="54">
         <v>8</v>
       </c>
       <c r="AG5" s="37" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AH5" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AI5" s="42"/>
       <c r="AJ5" s="37"/>
       <c r="AK5" s="37"/>
       <c r="AL5" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM5" s="37"/>
       <c r="AN5" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO5" s="20"/>
       <c r="AP5" s="20"/>
@@ -2742,13 +2732,13 @@
     </row>
     <row r="6" spans="1:64">
       <c r="A6" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>3</v>
@@ -2771,40 +2761,40 @@
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R6" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S6" s="31"/>
       <c r="T6" s="31"/>
       <c r="U6" s="31"/>
       <c r="V6" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W6" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X6" s="36"/>
       <c r="Y6" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z6" s="36"/>
       <c r="AA6" s="36"/>
       <c r="AB6" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AC6" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -2835,46 +2825,46 @@
     </row>
     <row r="7" spans="1:64">
       <c r="A7" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
@@ -2916,48 +2906,48 @@
     </row>
     <row r="8" spans="1:64">
       <c r="A8" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M8" s="31" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
       <c r="Q8" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S8" s="31"/>
       <c r="T8" s="31"/>
@@ -2966,19 +2956,19 @@
         <v>1</v>
       </c>
       <c r="W8" s="36" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="X8" s="36"/>
       <c r="Y8" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z8" s="47"/>
       <c r="AA8" s="36"/>
       <c r="AB8" s="36" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AC8" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD8" s="36"/>
       <c r="AE8" s="36"/>
@@ -3009,13 +2999,13 @@
     </row>
     <row r="9" spans="1:64">
       <c r="A9" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>3</v>
@@ -3038,52 +3028,52 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N9" s="31">
         <v>1</v>
       </c>
       <c r="O9" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T9" s="31">
         <v>45.244999999999997</v>
       </c>
       <c r="U9" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V9" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W9" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X9" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y9" s="43"/>
       <c r="Z9" s="43"/>
       <c r="AA9" s="36"/>
       <c r="AB9" s="36"/>
       <c r="AC9" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD9" s="29"/>
       <c r="AE9" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF9" s="37"/>
       <c r="AG9" s="37"/>
@@ -3112,13 +3102,13 @@
     </row>
     <row r="10" spans="1:64">
       <c r="A10" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>5</v>
@@ -3141,61 +3131,61 @@
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S10" s="31"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
       <c r="V10" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W10" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z10" s="36"/>
       <c r="AA10" s="36"/>
       <c r="AB10" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC10" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD10" s="29"/>
       <c r="AE10" s="29"/>
       <c r="AF10" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AG10" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH10" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI10" s="30"/>
       <c r="AJ10" s="37"/>
       <c r="AK10" s="37"/>
       <c r="AL10" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM10" s="30"/>
       <c r="AN10" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO10" s="20"/>
       <c r="AP10" s="20"/>
@@ -3215,48 +3205,48 @@
     </row>
     <row r="11" spans="1:64">
       <c r="A11" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
       <c r="Q11" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R11" s="31" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
@@ -3265,44 +3255,42 @@
         <v>2</v>
       </c>
       <c r="W11" s="36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="X11" s="36"/>
       <c r="Y11" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z11" s="36"/>
       <c r="AA11" s="36"/>
-      <c r="AB11" s="36" t="s">
-        <v>172</v>
-      </c>
+      <c r="AB11" s="36"/>
       <c r="AC11" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD11" s="29">
         <v>25.536000000000001</v>
       </c>
       <c r="AE11" s="48" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AF11" s="54">
         <v>12</v>
       </c>
       <c r="AG11" s="37" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AH11" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AI11" s="30"/>
       <c r="AJ11" s="37"/>
       <c r="AK11" s="37"/>
       <c r="AL11" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM11" s="30"/>
       <c r="AN11" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO11" s="20"/>
       <c r="AP11" s="20"/>
@@ -3322,13 +3310,13 @@
     </row>
     <row r="12" spans="1:64">
       <c r="A12" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>3</v>
@@ -3351,40 +3339,40 @@
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M12" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R12" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
       <c r="V12" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W12" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X12" s="36"/>
       <c r="Y12" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z12" s="36"/>
       <c r="AA12" s="36"/>
       <c r="AB12" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC12" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD12" s="29"/>
       <c r="AE12" s="29"/>
@@ -3415,13 +3403,13 @@
     </row>
     <row r="13" spans="1:64">
       <c r="A13" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>5</v>
@@ -3444,17 +3432,17 @@
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S13" s="31"/>
       <c r="T13" s="31"/>
@@ -3496,48 +3484,48 @@
     </row>
     <row r="14" spans="1:64">
       <c r="A14" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
       <c r="Q14" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
@@ -3546,19 +3534,19 @@
         <v>1</v>
       </c>
       <c r="W14" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X14" s="36"/>
       <c r="Y14" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z14" s="47"/>
       <c r="AA14" s="36"/>
       <c r="AB14" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AC14" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD14" s="36"/>
       <c r="AE14" s="36"/>
@@ -3589,13 +3577,13 @@
     </row>
     <row r="15" spans="1:64">
       <c r="A15" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>5</v>
@@ -3618,23 +3606,23 @@
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N15" s="31">
         <v>1</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P15" s="31"/>
       <c r="Q15" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S15" s="31"/>
       <c r="T15" s="31"/>
@@ -3676,13 +3664,13 @@
     </row>
     <row r="16" spans="1:64" ht="15" customHeight="1">
       <c r="A16" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>5</v>
@@ -3705,52 +3693,52 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N16" s="31">
         <v>1</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P16" s="31"/>
       <c r="Q16" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S16" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T16" s="31">
-        <v>38.331000000000003</v>
+        <v>16</v>
       </c>
       <c r="U16" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V16" s="49">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="W16" s="36" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="X16" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y16" s="36"/>
       <c r="Z16" s="36"/>
       <c r="AA16" s="36"/>
       <c r="AB16" s="36"/>
       <c r="AC16" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD16" s="36"/>
       <c r="AE16" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF16" s="37"/>
       <c r="AG16" s="37"/>
@@ -3779,81 +3767,81 @@
     </row>
     <row r="17" spans="1:64" ht="15" customHeight="1">
       <c r="A17" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="N17" s="31">
         <v>1</v>
       </c>
       <c r="O17" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P17" s="31"/>
       <c r="Q17" s="31" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="S17" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T17" s="31">
         <v>19.331</v>
       </c>
       <c r="U17" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V17" s="49">
         <v>11</v>
       </c>
       <c r="W17" s="36" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="X17" s="36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Y17" s="36"/>
       <c r="Z17" s="36"/>
       <c r="AA17" s="36"/>
       <c r="AB17" s="36"/>
       <c r="AC17" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD17" s="36"/>
       <c r="AE17" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF17" s="37"/>
       <c r="AG17" s="37"/>
@@ -3882,13 +3870,13 @@
     </row>
     <row r="18" spans="1:64" ht="13" customHeight="1">
       <c r="A18" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>32</v>
-      </c>
       <c r="C18" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>3</v>
@@ -3911,17 +3899,17 @@
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M18" s="31"/>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R18" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S18" s="31"/>
       <c r="T18" s="31"/>
@@ -3963,13 +3951,13 @@
     </row>
     <row r="19" spans="1:64">
       <c r="A19" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>5</v>
@@ -3992,17 +3980,17 @@
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R19" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S19" s="31"/>
       <c r="T19" s="31"/>
@@ -4044,48 +4032,48 @@
     </row>
     <row r="20" spans="1:64">
       <c r="A20" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R20" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S20" s="31"/>
       <c r="T20" s="31"/>
@@ -4094,19 +4082,17 @@
         <v>1</v>
       </c>
       <c r="W20" s="51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X20" s="51"/>
       <c r="Y20" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z20" s="52"/>
       <c r="AA20" s="51"/>
-      <c r="AB20" s="51" t="s">
-        <v>168</v>
-      </c>
+      <c r="AB20" s="51"/>
       <c r="AC20" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD20" s="36"/>
       <c r="AE20" s="36"/>
@@ -4137,13 +4123,13 @@
     </row>
     <row r="21" spans="1:64">
       <c r="A21" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>5</v>
@@ -4166,65 +4152,65 @@
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="31" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S21" s="31"/>
       <c r="T21" s="31"/>
       <c r="U21" s="31"/>
       <c r="V21" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W21" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X21" s="36"/>
       <c r="Y21" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z21" s="36"/>
       <c r="AA21" s="36"/>
       <c r="AB21" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC21" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD21" s="29">
-        <v>49.232999999999997</v>
+        <v>55</v>
       </c>
       <c r="AE21" s="48" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AF21" s="40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG21" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AH21" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI21" s="37"/>
       <c r="AJ21" s="37"/>
       <c r="AK21" s="37"/>
       <c r="AL21" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM21" s="30"/>
       <c r="AN21" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO21" s="44"/>
       <c r="AP21" s="17"/>
@@ -4246,13 +4232,13 @@
     </row>
     <row r="22" spans="1:64">
       <c r="A22" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="31" t="s">
-        <v>75</v>
-      </c>
       <c r="C22" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>5</v>
@@ -4275,40 +4261,40 @@
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S22" s="31"/>
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>
       <c r="V22" s="38" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="W22" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X22" s="36"/>
       <c r="Y22" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z22" s="36"/>
       <c r="AA22" s="36"/>
       <c r="AB22" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC22" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD22" s="29"/>
       <c r="AE22" s="29"/>
@@ -4340,52 +4326,52 @@
     </row>
     <row r="23" spans="1:64">
       <c r="A23" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>146</v>
-      </c>
       <c r="C23" s="33" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="N23" s="31">
         <v>1</v>
       </c>
       <c r="O23" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P23" s="31"/>
       <c r="Q23" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="S23" s="31"/>
       <c r="T23" s="31"/>
@@ -4428,13 +4414,13 @@
     </row>
     <row r="24" spans="1:64">
       <c r="A24" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="31" t="s">
-        <v>60</v>
-      </c>
       <c r="C24" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>5</v>
@@ -4457,52 +4443,52 @@
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="31" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="M24" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N24" s="31">
         <v>1</v>
       </c>
       <c r="O24" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P24" s="31"/>
       <c r="Q24" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S24" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T24" s="31">
-        <v>33.22</v>
+        <v>39</v>
       </c>
       <c r="U24" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V24" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W24" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X24" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y24" s="36"/>
       <c r="Z24" s="36"/>
       <c r="AA24" s="36"/>
       <c r="AB24" s="36"/>
       <c r="AC24" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD24" s="29"/>
       <c r="AE24" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF24" s="40"/>
       <c r="AG24" s="37"/>
@@ -4531,13 +4517,13 @@
     </row>
     <row r="25" spans="1:64">
       <c r="A25" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>5</v>
@@ -4560,65 +4546,65 @@
       <c r="J25" s="31"/>
       <c r="K25" s="31"/>
       <c r="L25" s="31" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N25" s="31"/>
       <c r="O25" s="31"/>
       <c r="P25" s="31"/>
       <c r="Q25" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S25" s="31"/>
       <c r="T25" s="31"/>
       <c r="U25" s="31"/>
       <c r="V25" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W25" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X25" s="36"/>
       <c r="Y25" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z25" s="36"/>
       <c r="AA25" s="36"/>
       <c r="AB25" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC25" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD25" s="29">
         <v>1.298</v>
       </c>
       <c r="AE25" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF25" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="AF25" s="40" t="s">
-        <v>104</v>
-      </c>
       <c r="AG25" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH25" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI25" s="30"/>
       <c r="AJ25" s="37"/>
       <c r="AK25" s="37"/>
       <c r="AL25" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM25" s="30"/>
       <c r="AN25" s="30" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AO25" s="44"/>
       <c r="AP25" s="20"/>
@@ -4638,81 +4624,81 @@
     </row>
     <row r="26" spans="1:64">
       <c r="A26" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
       <c r="L26" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N26" s="31">
         <v>1</v>
       </c>
       <c r="O26" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P26" s="31"/>
       <c r="Q26" s="31" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="S26" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T26" s="31">
         <v>55.5</v>
       </c>
       <c r="U26" s="55" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V26" s="53">
         <v>25</v>
       </c>
       <c r="W26" s="36" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="X26" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y26" s="36"/>
       <c r="Z26" s="36"/>
       <c r="AA26" s="36"/>
       <c r="AB26" s="36"/>
       <c r="AC26" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD26" s="29"/>
       <c r="AE26" s="29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AF26" s="40"/>
       <c r="AG26" s="37"/>
@@ -4741,13 +4727,13 @@
     </row>
     <row r="27" spans="1:64">
       <c r="A27" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" s="34" t="s">
         <v>5</v>
@@ -4770,40 +4756,40 @@
       <c r="J27" s="31"/>
       <c r="K27" s="31"/>
       <c r="L27" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N27" s="31"/>
       <c r="O27" s="31"/>
       <c r="P27" s="31"/>
       <c r="Q27" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S27" s="31"/>
       <c r="T27" s="31"/>
       <c r="U27" s="31"/>
       <c r="V27" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W27" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X27" s="36"/>
       <c r="Y27" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z27" s="36"/>
       <c r="AA27" s="36"/>
       <c r="AB27" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC27" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD27" s="29"/>
       <c r="AE27" s="29"/>
@@ -4834,11 +4820,11 @@
     </row>
     <row r="28" spans="1:64">
       <c r="A28" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="34" t="s">
         <v>5</v>
@@ -4862,13 +4848,13 @@
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
       <c r="M28" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N28" s="31"/>
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
       <c r="Q28" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>

</xml_diff>